<commit_message>
E works on allometric equations
</commit_message>
<xml_diff>
--- a/data/allometry/Isla_phd/Heights_Regression_Pika.xlsx
+++ b/data/allometry/Isla_phd/Heights_Regression_Pika.xlsx
@@ -1,20 +1,39 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="11113"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ericazaja/Desktop/Github_repos.tmp/NEW_MSC_ZAJA_2022/data/allometry/Isla_phd/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{07C53A6E-C99D-EF42-83AB-ED5D2AE6019A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="30" windowWidth="15315" windowHeight="7710"/>
+    <workbookView xWindow="5320" yWindow="1440" windowWidth="20880" windowHeight="13700" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="125725"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="58">
   <si>
     <t>Plot</t>
   </si>
@@ -161,16 +180,43 @@
   </si>
   <si>
     <t>day 14</t>
+  </si>
+  <si>
+    <t>Species</t>
+  </si>
+  <si>
+    <t>S. glauca, B. glandulosa</t>
+  </si>
+  <si>
+    <t>Salix pulchra</t>
+  </si>
+  <si>
+    <t>Salix pulchra??Betula</t>
+  </si>
+  <si>
+    <t>Salix richardsonii/pulchra or glauca or betula</t>
+  </si>
+  <si>
+    <t>Salix richardsonii/pulchra or glauca</t>
+  </si>
+  <si>
+    <t>Salix pulchra, or glauca or betula</t>
+  </si>
+  <si>
+    <t>Salix pulchra or rich or glauca or betula</t>
+  </si>
+  <si>
+    <t>Salix pulchra or rich</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="[Black]#,##0.00;[Red]\-#,##0.##"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -203,12 +249,24 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -224,48 +282,89 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="right"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyProtection="1">
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyProtection="1">
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
     <xf numFmtId="1" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="2" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 3" xfId="1"/>
+    <cellStyle name="Normal 3" xfId="1" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -312,7 +411,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -344,9 +443,27 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -378,6 +495,24 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -553,2929 +688,2699 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:AI102"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:AJ25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
+    <sheetView tabSelected="1" zoomScale="173" workbookViewId="0">
+      <selection activeCell="E19" sqref="E19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="23" width="9.140625" style="4"/>
-    <col min="24" max="25" width="9.140625" style="12"/>
-    <col min="26" max="31" width="9.140625" style="15"/>
-    <col min="32" max="16384" width="9.140625" style="4"/>
+    <col min="1" max="1" width="9.1640625" style="10"/>
+    <col min="2" max="3" width="9.1640625" style="3"/>
+    <col min="4" max="4" width="7.33203125" style="10" customWidth="1"/>
+    <col min="5" max="6" width="14.33203125" style="10" customWidth="1"/>
+    <col min="7" max="26" width="9.1640625" style="3"/>
+    <col min="27" max="32" width="9.1640625" style="8"/>
+    <col min="33" max="16384" width="9.1640625" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:35">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:36" x14ac:dyDescent="0.15">
+      <c r="A1" s="9" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="6" t="s">
+      <c r="C1" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="D1" s="6" t="s">
+      <c r="D1" s="11" t="s">
         <v>36</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="E1" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="F1" s="12" t="s">
+        <v>49</v>
+      </c>
+      <c r="G1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="H1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="I1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="J1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="J1" s="2" t="s">
+      <c r="K1" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="K1" s="2" t="s">
+      <c r="L1" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="L1" s="2" t="s">
+      <c r="M1" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="M1" s="2" t="s">
+      <c r="N1" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="N1" s="2" t="s">
+      <c r="O1" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="O1" s="2" t="s">
+      <c r="P1" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="P1" s="2" t="s">
+      <c r="Q1" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="Q1" s="2" t="s">
+      <c r="R1" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="R1" s="3" t="s">
+      <c r="S1" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="S1" s="3" t="s">
+      <c r="T1" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="T1" s="3" t="s">
+      <c r="U1" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="U1" s="3" t="s">
+      <c r="V1" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="V1" s="7" t="s">
+      <c r="W1" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="W1" s="7" t="s">
+      <c r="X1" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="X1" s="7" t="s">
+      <c r="Y1" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="Y1" s="7" t="s">
+      <c r="Z1" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="Z1" s="8" t="s">
+      <c r="AA1" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="AA1" s="9" t="s">
+      <c r="AB1" s="6" t="s">
         <v>41</v>
       </c>
-      <c r="AB1" s="8" t="s">
+      <c r="AC1" s="6" t="s">
         <v>42</v>
       </c>
-      <c r="AC1" s="8" t="s">
+      <c r="AD1" s="6" t="s">
         <v>43</v>
       </c>
-      <c r="AD1" s="8" t="s">
+      <c r="AE1" s="6" t="s">
         <v>44</v>
       </c>
-      <c r="AE1" s="8" t="s">
+      <c r="AF1" s="6" t="s">
         <v>45</v>
       </c>
-      <c r="AF1" s="4" t="s">
+      <c r="AG1" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="AG1" s="4" t="s">
+      <c r="AH1" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="AH1" s="4" t="s">
+      <c r="AI1" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="AI1" s="10"/>
+      <c r="AJ1" s="7"/>
     </row>
-    <row r="2" spans="1:35">
-      <c r="A2" s="1" t="s">
+    <row r="2" spans="1:36" s="16" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A2" s="13" t="s">
         <v>19</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B2" s="13" t="s">
         <v>20</v>
       </c>
-      <c r="C2" s="6">
+      <c r="C2" s="14">
         <v>3.3662962962962966</v>
       </c>
-      <c r="D2" s="6">
+      <c r="D2" s="14">
         <v>2050</v>
       </c>
-      <c r="E2" s="5">
+      <c r="E2" s="15">
         <v>49</v>
       </c>
-      <c r="F2" s="5">
+      <c r="F2" s="15" t="s">
+        <v>50</v>
+      </c>
+      <c r="G2" s="15">
         <v>0</v>
       </c>
-      <c r="G2" s="5">
+      <c r="H2" s="15">
         <v>0.94267206477732801</v>
       </c>
-      <c r="H2" s="5">
+      <c r="I2" s="15">
         <v>8.06666666666667</v>
       </c>
-      <c r="I2" s="5">
+      <c r="J2" s="15">
         <v>14</v>
       </c>
-      <c r="J2" s="5">
+      <c r="K2" s="15">
         <v>41.159500000000001</v>
       </c>
-      <c r="K2" s="5">
+      <c r="L2" s="15">
         <v>75</v>
       </c>
-      <c r="L2" s="5">
+      <c r="M2" s="15">
         <v>-8.6633766801075307</v>
       </c>
-      <c r="M2" s="5">
+      <c r="N2" s="15">
         <v>7.7634873431899596</v>
       </c>
-      <c r="N2" s="5">
+      <c r="O2" s="15">
         <v>37</v>
       </c>
-      <c r="O2" s="5">
+      <c r="P2" s="15">
         <v>57.284500000000001</v>
       </c>
-      <c r="P2" s="5">
+      <c r="Q2" s="15">
         <v>39.668999999999997</v>
       </c>
-      <c r="Q2" s="5">
+      <c r="R2" s="15">
         <v>8.5</v>
       </c>
-      <c r="R2" s="4">
+      <c r="S2" s="16">
         <v>0.19020000000000001</v>
       </c>
-      <c r="S2" s="4">
+      <c r="T2" s="16">
         <v>7.1850000000000025E-2</v>
       </c>
-      <c r="T2" s="4">
+      <c r="U2" s="16">
         <v>0.2102</v>
       </c>
-      <c r="U2" s="4">
+      <c r="V2" s="16">
         <v>0.32285000000000003</v>
       </c>
-      <c r="V2" s="11">
+      <c r="W2" s="17">
         <v>1.895</v>
       </c>
-      <c r="W2" s="11">
+      <c r="X2" s="17">
         <v>49.03</v>
       </c>
-      <c r="X2" s="12">
+      <c r="Y2" s="16">
         <v>1.9350000000000001</v>
       </c>
-      <c r="Y2" s="12">
+      <c r="Z2" s="16">
         <v>47.784999999999997</v>
       </c>
-      <c r="Z2" s="13">
+      <c r="AA2" s="18">
         <v>11.2</v>
       </c>
-      <c r="AA2" s="14">
+      <c r="AB2" s="19">
         <v>0.8</v>
       </c>
-      <c r="AB2" s="13">
+      <c r="AC2" s="18">
         <v>10.4</v>
       </c>
-      <c r="AC2" s="8">
+      <c r="AD2" s="20">
         <v>13.5</v>
       </c>
-      <c r="AD2" s="8">
+      <c r="AE2" s="20">
         <v>5.3</v>
       </c>
-      <c r="AE2" s="8">
+      <c r="AF2" s="20">
         <v>8.1999999999999993</v>
       </c>
-      <c r="AF2" s="4">
+      <c r="AG2" s="16">
         <v>1.4700000000000002</v>
       </c>
-      <c r="AG2" s="4">
+      <c r="AH2" s="16">
         <v>0.14249999999999963</v>
       </c>
-      <c r="AH2" s="4">
+      <c r="AI2" s="16">
         <v>0.16249999999999964</v>
       </c>
     </row>
-    <row r="3" spans="1:35">
-      <c r="A3" s="1" t="s">
+    <row r="3" spans="1:36" s="24" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A3" s="21" t="s">
         <v>21</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="B3" s="21" t="s">
         <v>20</v>
       </c>
-      <c r="C3" s="6">
+      <c r="C3" s="22">
         <v>1.335574074074074</v>
       </c>
-      <c r="D3" s="6">
+      <c r="D3" s="22">
         <v>1850</v>
       </c>
-      <c r="E3" s="5">
+      <c r="E3" s="23">
         <v>62.5</v>
       </c>
-      <c r="F3" s="5">
+      <c r="F3" s="24" t="s">
+        <v>51</v>
+      </c>
+      <c r="G3" s="23">
         <v>0</v>
       </c>
-      <c r="G3" s="5">
+      <c r="H3" s="23">
         <v>0.650482365965523</v>
       </c>
-      <c r="H3" s="5">
+      <c r="I3" s="23">
         <v>4</v>
       </c>
-      <c r="I3" s="5">
+      <c r="J3" s="23">
         <v>72</v>
       </c>
-      <c r="J3" s="5">
+      <c r="K3" s="23">
         <v>48.061500000000002</v>
       </c>
-      <c r="K3" s="5">
+      <c r="L3" s="23">
         <v>75</v>
       </c>
-      <c r="L3" s="5">
+      <c r="M3" s="23">
         <v>-2.3229530689964202</v>
       </c>
-      <c r="M3" s="5">
+      <c r="N3" s="23">
         <v>8.7349324596774203</v>
       </c>
-      <c r="N3" s="5">
+      <c r="O3" s="23">
         <v>46.870967741935502</v>
       </c>
-      <c r="O3" s="5">
+      <c r="P3" s="23">
         <v>88.254499999999993</v>
       </c>
-      <c r="P3" s="5">
+      <c r="Q3" s="23">
         <v>52.7575</v>
       </c>
-      <c r="Q3" s="5">
+      <c r="R3" s="23">
         <v>10.25</v>
       </c>
-      <c r="R3" s="4">
+      <c r="S3" s="24">
         <v>0.21880000000000002</v>
       </c>
-      <c r="S3" s="4">
+      <c r="T3" s="24">
         <v>2.1600000000000008E-2</v>
       </c>
-      <c r="T3" s="4">
+      <c r="U3" s="24">
         <v>0.14365</v>
       </c>
-      <c r="U3" s="4">
+      <c r="V3" s="24">
         <v>0.13040000000000002</v>
       </c>
-      <c r="V3" s="11">
+      <c r="W3" s="25">
         <v>1.72</v>
       </c>
-      <c r="W3" s="11">
+      <c r="X3" s="25">
         <v>48.519999999999996</v>
       </c>
-      <c r="X3" s="12">
+      <c r="Y3" s="24">
         <v>1.7650000000000001</v>
       </c>
-      <c r="Y3" s="12">
+      <c r="Z3" s="24">
         <v>45.174999999999997</v>
       </c>
-      <c r="Z3" s="13">
+      <c r="AA3" s="26">
         <v>6.2</v>
       </c>
-      <c r="AA3" s="14">
+      <c r="AB3" s="27">
         <v>1.6</v>
       </c>
-      <c r="AB3" s="13">
+      <c r="AC3" s="26">
         <v>4.5999999999999996</v>
       </c>
-      <c r="AC3" s="8">
+      <c r="AD3" s="28">
         <v>16.100000000000001</v>
       </c>
-      <c r="AD3" s="8">
+      <c r="AE3" s="28">
         <v>6.1</v>
       </c>
-      <c r="AE3" s="8">
+      <c r="AF3" s="28">
         <v>10</v>
       </c>
-      <c r="AF3" s="4">
+      <c r="AG3" s="24">
         <v>1.5775000000000003</v>
       </c>
-      <c r="AG3" s="4">
+      <c r="AH3" s="24">
         <v>0.15249999999999986</v>
       </c>
-      <c r="AH3" s="4">
+      <c r="AI3" s="24">
         <v>0.11000000000000032</v>
       </c>
     </row>
-    <row r="4" spans="1:35">
-      <c r="A4" s="1" t="s">
+    <row r="4" spans="1:36" s="24" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A4" s="21" t="s">
         <v>22</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="B4" s="21" t="s">
         <v>20</v>
       </c>
-      <c r="C4" s="6">
+      <c r="C4" s="22">
         <v>1.0972962962962962</v>
       </c>
-      <c r="D4" s="6">
+      <c r="D4" s="22">
         <v>1247.5</v>
       </c>
-      <c r="E4" s="5">
+      <c r="E4" s="23">
         <v>72.5</v>
       </c>
-      <c r="F4" s="5">
+      <c r="F4" s="23" t="s">
+        <v>53</v>
+      </c>
+      <c r="G4" s="23">
         <v>80</v>
       </c>
-      <c r="G4" s="5">
+      <c r="H4" s="23">
         <v>0.95971310849992397</v>
       </c>
-      <c r="H4" s="5">
+      <c r="I4" s="23">
         <v>4.2666666666666702</v>
       </c>
-      <c r="I4" s="5">
+      <c r="J4" s="23">
         <v>19.6666666666667</v>
       </c>
-      <c r="J4" s="5">
+      <c r="K4" s="23">
         <v>40.798499999999997</v>
       </c>
-      <c r="K4" s="5">
+      <c r="L4" s="23">
         <v>37.5</v>
       </c>
-      <c r="L4" s="5">
+      <c r="M4" s="23">
         <v>-3.51526792114695</v>
       </c>
-      <c r="M4" s="5">
+      <c r="N4" s="23">
         <v>4.3894958557347596</v>
       </c>
-      <c r="N4" s="5">
+      <c r="O4" s="23">
         <v>27.4838709677419</v>
       </c>
-      <c r="O4" s="5">
+      <c r="P4" s="23">
         <v>137.279</v>
       </c>
-      <c r="P4" s="5">
+      <c r="Q4" s="23">
         <v>53.256</v>
       </c>
-      <c r="Q4" s="5">
+      <c r="R4" s="23">
         <v>11.5</v>
       </c>
-      <c r="R4" s="4">
+      <c r="S4" s="24">
         <v>0.20140000000000002</v>
       </c>
-      <c r="S4" s="4">
+      <c r="T4" s="24">
         <v>4.6350000000000002E-2</v>
       </c>
-      <c r="T4" s="4">
+      <c r="U4" s="24">
         <v>0.20754999999999998</v>
       </c>
-      <c r="U4" s="4">
+      <c r="V4" s="24">
         <v>0.30865000000000004</v>
       </c>
-      <c r="V4" s="11">
+      <c r="W4" s="25">
         <v>1.7549999999999999</v>
       </c>
-      <c r="W4" s="11">
+      <c r="X4" s="25">
         <v>48.894999999999996</v>
       </c>
-      <c r="X4" s="12">
+      <c r="Y4" s="24">
         <v>1.9350000000000001</v>
       </c>
-      <c r="Y4" s="12">
+      <c r="Z4" s="24">
         <v>48.16</v>
       </c>
-      <c r="Z4" s="13">
+      <c r="AA4" s="26">
         <v>6.6</v>
       </c>
-      <c r="AA4" s="14">
+      <c r="AB4" s="27">
         <v>1.6</v>
       </c>
-      <c r="AB4" s="13">
+      <c r="AC4" s="26">
         <v>5</v>
       </c>
-      <c r="AC4" s="8">
+      <c r="AD4" s="28">
         <v>12.899999999999999</v>
       </c>
-      <c r="AD4" s="8">
+      <c r="AE4" s="28">
         <v>3.1999999999999997</v>
       </c>
-      <c r="AE4" s="8">
+      <c r="AF4" s="28">
         <v>9.6999999999999993</v>
       </c>
-      <c r="AF4" s="4">
+      <c r="AG4" s="24">
         <v>1.1200000000000001</v>
       </c>
-      <c r="AG4" s="4">
+      <c r="AH4" s="24">
         <v>0.19500000000000028</v>
       </c>
-      <c r="AH4" s="4">
+      <c r="AI4" s="24">
         <v>0.1875</v>
       </c>
     </row>
-    <row r="5" spans="1:35">
-      <c r="A5" s="1" t="s">
+    <row r="5" spans="1:36" s="24" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A5" s="21" t="s">
         <v>23</v>
       </c>
-      <c r="B5" s="1" t="s">
+      <c r="B5" s="21" t="s">
         <v>20</v>
       </c>
-      <c r="C5" s="6">
+      <c r="C5" s="22">
         <v>3.9551851851851847</v>
       </c>
-      <c r="D5" s="6">
+      <c r="D5" s="22">
         <v>1575</v>
       </c>
-      <c r="E5" s="5">
+      <c r="E5" s="23">
         <v>71.5</v>
       </c>
-      <c r="F5" s="5">
+      <c r="F5" s="23" t="s">
+        <v>55</v>
+      </c>
+      <c r="G5" s="23">
         <v>0</v>
       </c>
-      <c r="G5" s="5">
+      <c r="H5" s="23">
         <v>0.927032552288096</v>
       </c>
-      <c r="H5" s="5">
+      <c r="I5" s="23">
         <v>7.8666666666666698</v>
       </c>
-      <c r="I5" s="5">
+      <c r="J5" s="23">
         <v>14</v>
       </c>
-      <c r="J5" s="5">
+      <c r="K5" s="23">
         <v>45.463000000000001</v>
       </c>
-      <c r="K5" s="5">
+      <c r="L5" s="23">
         <v>50</v>
       </c>
-      <c r="L5" s="5">
+      <c r="M5" s="23">
         <v>-6.0453319892473099</v>
       </c>
-      <c r="M5" s="5">
+      <c r="N5" s="23">
         <v>9.9609489247311807</v>
       </c>
-      <c r="N5" s="5">
+      <c r="O5" s="23">
         <v>28.322580645161299</v>
       </c>
-      <c r="O5" s="5">
+      <c r="P5" s="23">
         <v>31.433499999999999</v>
       </c>
-      <c r="P5" s="5">
+      <c r="Q5" s="23">
         <v>3.1764999999999999</v>
       </c>
-      <c r="Q5" s="5">
+      <c r="R5" s="23">
         <v>5.45</v>
       </c>
-      <c r="R5" s="4">
+      <c r="S5" s="24">
         <v>0.24875</v>
       </c>
-      <c r="S5" s="4">
+      <c r="T5" s="24">
         <v>2.0650000000000029E-2</v>
       </c>
-      <c r="T5" s="4">
+      <c r="U5" s="24">
         <v>0.26775000000000004</v>
       </c>
-      <c r="U5" s="4">
+      <c r="V5" s="24">
         <v>0.35020000000000001</v>
       </c>
-      <c r="V5" s="11">
+      <c r="W5" s="25">
         <v>2.1349999999999998</v>
       </c>
-      <c r="W5" s="11">
+      <c r="X5" s="25">
         <v>48.335000000000001</v>
       </c>
-      <c r="X5" s="12">
+      <c r="Y5" s="24">
         <v>2.3199999999999998</v>
       </c>
-      <c r="Y5" s="12">
+      <c r="Z5" s="24">
         <v>47</v>
       </c>
-      <c r="Z5" s="13">
+      <c r="AA5" s="26">
         <v>9</v>
       </c>
-      <c r="AA5" s="14">
+      <c r="AB5" s="27">
         <v>2.8</v>
       </c>
-      <c r="AB5" s="13">
+      <c r="AC5" s="26">
         <v>6.2</v>
       </c>
-      <c r="AC5" s="8">
+      <c r="AD5" s="28">
         <v>15.100000000000001</v>
       </c>
-      <c r="AD5" s="8">
+      <c r="AE5" s="28">
         <v>6.2</v>
       </c>
-      <c r="AE5" s="8">
+      <c r="AF5" s="28">
         <v>8.9</v>
       </c>
-      <c r="AF5" s="4">
+      <c r="AG5" s="24">
         <v>1.3400000000000003</v>
       </c>
-      <c r="AG5" s="4">
+      <c r="AH5" s="24">
         <v>0.23249999999999993</v>
       </c>
-      <c r="AH5" s="4">
+      <c r="AI5" s="24">
         <v>0.2475000000000005</v>
       </c>
     </row>
-    <row r="6" spans="1:35">
-      <c r="A6" s="1" t="s">
+    <row r="6" spans="1:36" s="24" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A6" s="21" t="s">
         <v>24</v>
       </c>
-      <c r="B6" s="1" t="s">
+      <c r="B6" s="21" t="s">
         <v>20</v>
       </c>
-      <c r="C6" s="6">
+      <c r="C6" s="22">
         <v>1.4217407407407407</v>
       </c>
-      <c r="D6" s="6">
+      <c r="D6" s="22">
         <v>1372.5</v>
       </c>
-      <c r="E6" s="5">
+      <c r="E6" s="23">
         <v>60</v>
       </c>
-      <c r="F6" s="5">
+      <c r="F6" s="23" t="s">
+        <v>57</v>
+      </c>
+      <c r="G6" s="23">
         <v>72.5</v>
       </c>
-      <c r="G6" s="5">
+      <c r="H6" s="23">
         <v>0.93346205257685999</v>
       </c>
-      <c r="H6" s="5">
+      <c r="I6" s="23">
         <v>11.0666666666667</v>
       </c>
-      <c r="I6" s="5">
+      <c r="J6" s="23">
         <v>34.6666666666667</v>
       </c>
-      <c r="J6" s="5">
+      <c r="K6" s="23">
         <v>47.109499999999997</v>
       </c>
-      <c r="K6" s="5">
+      <c r="L6" s="23">
         <v>37.5</v>
       </c>
-      <c r="L6" s="5">
+      <c r="M6" s="23">
         <v>-6.8891883960573503</v>
       </c>
-      <c r="M6" s="5">
+      <c r="N6" s="23">
         <v>8.0656491935483903</v>
       </c>
-      <c r="N6" s="5">
+      <c r="O6" s="23">
         <v>19.209677419354801</v>
       </c>
-      <c r="O6" s="5">
+      <c r="P6" s="23">
         <v>225.67400000000001</v>
       </c>
-      <c r="P6" s="5">
+      <c r="Q6" s="23">
         <v>186.50299999999999</v>
       </c>
-      <c r="Q6" s="5">
+      <c r="R6" s="23">
         <v>20.45</v>
       </c>
-      <c r="R6" s="4">
+      <c r="S6" s="24">
         <v>0.21095</v>
       </c>
-      <c r="S6" s="4">
+      <c r="T6" s="24">
         <v>2.5900000000000006E-2</v>
       </c>
-      <c r="T6" s="4">
+      <c r="U6" s="24">
         <v>0.22115000000000001</v>
       </c>
-      <c r="U6" s="4">
+      <c r="V6" s="24">
         <v>0.30065000000000003</v>
       </c>
-      <c r="V6" s="11">
+      <c r="W6" s="25">
         <v>1.7749999999999999</v>
       </c>
-      <c r="W6" s="11">
+      <c r="X6" s="25">
         <v>49.46</v>
       </c>
-      <c r="X6" s="12">
+      <c r="Y6" s="24">
         <v>2.09</v>
       </c>
-      <c r="Y6" s="12">
+      <c r="Z6" s="24">
         <v>49.08</v>
       </c>
-      <c r="Z6" s="13">
+      <c r="AA6" s="26">
         <v>5.8</v>
       </c>
-      <c r="AA6" s="14">
+      <c r="AB6" s="27">
         <v>1.6</v>
       </c>
-      <c r="AB6" s="13">
+      <c r="AC6" s="26">
         <v>4.2</v>
       </c>
-      <c r="AC6" s="8">
+      <c r="AD6" s="28">
         <v>16.100000000000001</v>
       </c>
-      <c r="AD6" s="8">
+      <c r="AE6" s="28">
         <v>7.5</v>
       </c>
-      <c r="AE6" s="8">
+      <c r="AF6" s="28">
         <v>8.6</v>
       </c>
-      <c r="AF6" s="4">
+      <c r="AG6" s="24">
         <v>0.75749999999999984</v>
       </c>
-      <c r="AG6" s="4">
+      <c r="AH6" s="24">
         <v>0.10749999999999993</v>
       </c>
-      <c r="AH6" s="4">
+      <c r="AI6" s="24">
         <v>0.15249999999999986</v>
       </c>
     </row>
-    <row r="7" spans="1:35">
-      <c r="A7" s="1" t="s">
+    <row r="7" spans="1:36" s="24" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A7" s="21" t="s">
         <v>25</v>
       </c>
-      <c r="B7" s="1" t="s">
+      <c r="B7" s="21" t="s">
         <v>20</v>
       </c>
-      <c r="C7" s="6">
+      <c r="C7" s="22">
         <v>1.7906296296296296</v>
       </c>
-      <c r="D7" s="6">
+      <c r="D7" s="22">
         <v>970</v>
       </c>
-      <c r="E7" s="5">
+      <c r="E7" s="23">
         <v>75</v>
       </c>
-      <c r="F7" s="5">
+      <c r="F7" s="23" t="s">
+        <v>51</v>
+      </c>
+      <c r="G7" s="23">
         <v>0</v>
       </c>
-      <c r="G7" s="5">
+      <c r="H7" s="23">
         <v>0.94923537758158605</v>
       </c>
-      <c r="H7" s="5">
+      <c r="I7" s="23">
         <v>10.9</v>
       </c>
-      <c r="I7" s="5">
+      <c r="J7" s="23">
         <v>16.3333333333333</v>
       </c>
-      <c r="J7" s="5">
+      <c r="K7" s="23">
         <v>57.390500000000003</v>
       </c>
-      <c r="K7" s="5">
+      <c r="L7" s="23">
         <v>50</v>
       </c>
-      <c r="L7" s="5">
+      <c r="M7" s="23">
         <v>-6.4921092069892499</v>
       </c>
-      <c r="M7" s="5">
+      <c r="N7" s="23">
         <v>5.2231011424731202</v>
       </c>
-      <c r="N7" s="5">
+      <c r="O7" s="23">
         <v>22.2258064516129</v>
       </c>
-      <c r="O7" s="5">
+      <c r="P7" s="23">
         <v>105.889</v>
       </c>
-      <c r="P7" s="5">
+      <c r="Q7" s="23">
         <v>41.467500000000001</v>
       </c>
-      <c r="Q7" s="5">
+      <c r="R7" s="23">
         <v>19.25</v>
       </c>
-      <c r="R7" s="4">
+      <c r="S7" s="24">
         <v>0.23</v>
       </c>
-      <c r="S7" s="4">
+      <c r="T7" s="24">
         <v>1.5199999999999991E-2</v>
       </c>
-      <c r="T7" s="4">
+      <c r="U7" s="24">
         <v>0.23760000000000001</v>
       </c>
-      <c r="U7" s="4">
+      <c r="V7" s="24">
         <v>0.25770000000000004</v>
       </c>
-      <c r="V7" s="11">
+      <c r="W7" s="25">
         <v>1.79</v>
       </c>
-      <c r="W7" s="11">
+      <c r="X7" s="25">
         <v>49.064999999999998</v>
       </c>
-      <c r="X7" s="12">
+      <c r="Y7" s="24">
         <v>1.99</v>
       </c>
-      <c r="Y7" s="12">
+      <c r="Z7" s="24">
         <v>47.05</v>
       </c>
-      <c r="Z7" s="13">
+      <c r="AA7" s="26">
         <v>9.1999999999999993</v>
       </c>
-      <c r="AA7" s="14">
+      <c r="AB7" s="27">
         <v>4.8</v>
       </c>
-      <c r="AB7" s="13">
+      <c r="AC7" s="26">
         <v>4.4000000000000004</v>
       </c>
-      <c r="AC7" s="8">
+      <c r="AD7" s="28">
         <v>15.4</v>
       </c>
-      <c r="AD7" s="8">
+      <c r="AE7" s="28">
         <v>6.6</v>
       </c>
-      <c r="AE7" s="8">
+      <c r="AF7" s="28">
         <v>8.8000000000000007</v>
       </c>
-      <c r="AF7" s="4">
+      <c r="AG7" s="24">
         <v>1.5525</v>
       </c>
-      <c r="AG7" s="4">
+      <c r="AH7" s="24">
         <v>0.20249999999999968</v>
       </c>
-      <c r="AH7" s="4">
+      <c r="AI7" s="24">
         <v>0.16250000000000009</v>
       </c>
     </row>
-    <row r="8" spans="1:35">
-      <c r="A8" s="1" t="s">
+    <row r="8" spans="1:36" s="16" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A8" s="13" t="s">
         <v>19</v>
       </c>
-      <c r="B8" s="1" t="s">
+      <c r="B8" s="13" t="s">
         <v>26</v>
       </c>
-      <c r="C8" s="6">
+      <c r="C8" s="14">
         <v>1.4415555555555557</v>
       </c>
-      <c r="D8" s="6">
+      <c r="D8" s="14">
         <v>772.5</v>
       </c>
-      <c r="E8" s="5">
+      <c r="E8" s="15">
         <v>56.5</v>
       </c>
-      <c r="F8" s="5">
+      <c r="F8" s="15" t="s">
+        <v>50</v>
+      </c>
+      <c r="G8" s="15">
         <v>34.5</v>
       </c>
-      <c r="G8" s="5">
+      <c r="H8" s="15">
         <v>0</v>
       </c>
-      <c r="H8" s="5">
+      <c r="I8" s="15">
         <v>8.3333333333333304</v>
       </c>
-      <c r="I8" s="5">
+      <c r="J8" s="15">
         <v>17.6666666666667</v>
       </c>
-      <c r="J8" s="5">
+      <c r="K8" s="15">
         <v>68.150000000000006</v>
       </c>
-      <c r="K8" s="5">
+      <c r="L8" s="15">
         <v>25</v>
       </c>
-      <c r="L8" s="5">
+      <c r="M8" s="15">
         <v>-8.04379816308243</v>
       </c>
-      <c r="M8" s="5">
+      <c r="N8" s="15">
         <v>9.7272843862007203</v>
       </c>
-      <c r="N8" s="5">
+      <c r="O8" s="15">
         <v>12.677419354838699</v>
       </c>
-      <c r="O8" s="5">
+      <c r="P8" s="15">
         <v>111.20650000000001</v>
       </c>
-      <c r="P8" s="5">
+      <c r="Q8" s="15">
         <v>14.3375</v>
       </c>
-      <c r="Q8" s="5">
+      <c r="R8" s="15">
         <v>20.65</v>
       </c>
-      <c r="R8" s="4">
+      <c r="S8" s="16">
         <v>0.21315000000000001</v>
       </c>
-      <c r="S8" s="4">
+      <c r="T8" s="16">
         <v>3.0950000000000005E-2</v>
       </c>
-      <c r="T8" s="4">
+      <c r="U8" s="16">
         <v>0.20519999999999999</v>
       </c>
-      <c r="U8" s="4">
+      <c r="V8" s="16">
         <v>0.19690000000000002</v>
       </c>
-      <c r="V8" s="11">
+      <c r="W8" s="17">
         <v>1.665</v>
       </c>
-      <c r="W8" s="11">
+      <c r="X8" s="17">
         <v>48.924999999999997</v>
       </c>
-      <c r="X8" s="12">
+      <c r="Y8" s="16">
         <v>1.93</v>
       </c>
-      <c r="Y8" s="12">
+      <c r="Z8" s="16">
         <v>48.01</v>
       </c>
-      <c r="Z8" s="13">
+      <c r="AA8" s="18">
         <v>11.6</v>
       </c>
-      <c r="AA8" s="14">
+      <c r="AB8" s="19">
         <v>1</v>
       </c>
-      <c r="AB8" s="13">
+      <c r="AC8" s="18">
         <v>10.6</v>
       </c>
-      <c r="AC8" s="8">
+      <c r="AD8" s="20">
         <v>10.7</v>
       </c>
-      <c r="AD8" s="8">
+      <c r="AE8" s="20">
         <v>3.6</v>
       </c>
-      <c r="AE8" s="8">
+      <c r="AF8" s="20">
         <v>7.1</v>
       </c>
-      <c r="AF8" s="4">
+      <c r="AG8" s="16">
         <v>1.5649999999999999</v>
       </c>
-      <c r="AG8" s="4">
+      <c r="AH8" s="16">
         <v>0.42999999999999972</v>
       </c>
-      <c r="AH8" s="4">
+      <c r="AI8" s="16">
         <v>0.15000000000000036</v>
       </c>
     </row>
-    <row r="9" spans="1:35">
-      <c r="A9" s="1" t="s">
+    <row r="9" spans="1:36" s="24" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A9" s="21" t="s">
         <v>21</v>
       </c>
-      <c r="B9" s="1" t="s">
+      <c r="B9" s="21" t="s">
         <v>26</v>
       </c>
-      <c r="C9" s="6">
+      <c r="C9" s="22">
         <v>3.2866666666666666</v>
       </c>
-      <c r="D9" s="6">
+      <c r="D9" s="22">
         <v>417.5</v>
       </c>
-      <c r="E9" s="4">
+      <c r="E9" s="24">
         <v>0</v>
       </c>
-      <c r="F9" s="5">
+      <c r="F9" s="24" t="s">
+        <v>51</v>
+      </c>
+      <c r="G9" s="23">
         <v>200</v>
       </c>
-      <c r="G9" s="5">
+      <c r="H9" s="23">
         <v>0.16557768924302799</v>
       </c>
-      <c r="H9" s="5">
+      <c r="I9" s="23">
         <v>7.9666666666666703</v>
       </c>
-      <c r="I9" s="5">
+      <c r="J9" s="23">
         <v>20.6666666666667</v>
       </c>
-      <c r="J9" s="5">
+      <c r="K9" s="23">
         <v>72.4345</v>
       </c>
-      <c r="K9" s="5">
+      <c r="L9" s="23">
         <v>17.5</v>
       </c>
-      <c r="L9" s="5">
+      <c r="M9" s="23">
         <v>-8.4800591893817199</v>
       </c>
-      <c r="M9" s="5">
+      <c r="N9" s="23">
         <v>10.087756973196701</v>
       </c>
-      <c r="N9" s="5">
+      <c r="O9" s="23">
         <v>6.1451612903225801</v>
       </c>
-      <c r="O9" s="5">
+      <c r="P9" s="23">
         <v>98.052000000000007</v>
       </c>
-      <c r="P9" s="5">
+      <c r="Q9" s="23">
         <v>1.5175000000000001</v>
       </c>
-      <c r="Q9" s="5">
+      <c r="R9" s="23">
         <v>17.05</v>
       </c>
-      <c r="R9" s="4">
+      <c r="S9" s="24">
         <v>0.1812</v>
       </c>
-      <c r="S9" s="4">
+      <c r="T9" s="24">
         <v>2.6499999999999996E-2</v>
       </c>
-      <c r="T9" s="4">
+      <c r="U9" s="24">
         <v>0.21359999999999998</v>
       </c>
-      <c r="U9" s="4">
+      <c r="V9" s="24">
         <v>0.22460000000000002</v>
       </c>
-      <c r="V9" s="11">
+      <c r="W9" s="25">
         <v>1.6600000000000001</v>
       </c>
-      <c r="W9" s="11">
+      <c r="X9" s="25">
         <v>49.385000000000005</v>
       </c>
-      <c r="X9" s="12">
+      <c r="Y9" s="24">
         <v>1.9450000000000001</v>
       </c>
-      <c r="Y9" s="12">
+      <c r="Z9" s="24">
         <v>49.495000000000005</v>
       </c>
-      <c r="Z9" s="13">
+      <c r="AA9" s="26">
         <v>10.4</v>
       </c>
-      <c r="AA9" s="14">
+      <c r="AB9" s="27">
         <v>1.6</v>
       </c>
-      <c r="AB9" s="13">
+      <c r="AC9" s="26">
         <v>8.8000000000000007</v>
       </c>
-      <c r="AC9" s="8">
+      <c r="AD9" s="28">
         <v>10</v>
       </c>
-      <c r="AD9" s="8">
+      <c r="AE9" s="28">
         <v>2.1</v>
       </c>
-      <c r="AE9" s="8">
+      <c r="AF9" s="28">
         <v>7.9</v>
       </c>
-      <c r="AF9" s="4">
+      <c r="AG9" s="24">
         <v>1.7999999999999998</v>
       </c>
-      <c r="AG9" s="4">
+      <c r="AH9" s="24">
         <v>0.24500000000000011</v>
       </c>
-      <c r="AH9" s="4">
+      <c r="AI9" s="24">
         <v>0.20500000000000007</v>
       </c>
     </row>
-    <row r="10" spans="1:35">
-      <c r="A10" s="1" t="s">
+    <row r="10" spans="1:36" s="24" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A10" s="21" t="s">
         <v>22</v>
       </c>
-      <c r="B10" s="1" t="s">
+      <c r="B10" s="21" t="s">
         <v>26</v>
       </c>
-      <c r="C10" s="6">
+      <c r="C10" s="22">
         <v>1.8455555555555554</v>
       </c>
-      <c r="D10" s="6">
+      <c r="D10" s="22">
         <v>1177.5</v>
       </c>
-      <c r="E10" s="5">
+      <c r="E10" s="23">
         <v>47.5</v>
       </c>
-      <c r="F10" s="5">
+      <c r="F10" s="23" t="s">
+        <v>53</v>
+      </c>
+      <c r="G10" s="23">
         <v>23.5</v>
       </c>
-      <c r="G10" s="5">
+      <c r="H10" s="23">
         <v>5.1214606220021698E-2</v>
       </c>
-      <c r="H10" s="5">
+      <c r="I10" s="23">
         <v>6.7333333333333298</v>
       </c>
-      <c r="I10" s="5">
+      <c r="J10" s="23">
         <v>55.6666666666667</v>
       </c>
-      <c r="J10" s="5">
+      <c r="K10" s="23">
         <v>43.338500000000003</v>
       </c>
-      <c r="K10" s="5">
+      <c r="L10" s="23">
         <v>25</v>
       </c>
-      <c r="L10" s="5">
+      <c r="M10" s="23">
         <v>-7.7283195564516101</v>
       </c>
-      <c r="M10" s="5">
+      <c r="N10" s="23">
         <v>10.737940748207899</v>
       </c>
-      <c r="N10" s="5">
+      <c r="O10" s="23">
         <v>11.6290322580645</v>
       </c>
-      <c r="O10" s="5">
+      <c r="P10" s="23">
         <v>111.711</v>
       </c>
-      <c r="P10" s="5">
+      <c r="Q10" s="23">
         <v>14.159000000000001</v>
       </c>
-      <c r="Q10" s="5">
+      <c r="R10" s="23">
         <v>14.25</v>
       </c>
-      <c r="R10" s="4">
+      <c r="S10" s="24">
         <v>0.1724</v>
       </c>
-      <c r="S10" s="4">
+      <c r="T10" s="24">
         <v>5.0850000000000006E-2</v>
       </c>
-      <c r="T10" s="4">
+      <c r="U10" s="24">
         <v>0.2044</v>
       </c>
-      <c r="U10" s="4">
+      <c r="V10" s="24">
         <v>0.22664999999999999</v>
       </c>
-      <c r="V10" s="11">
+      <c r="W10" s="25">
         <v>1.8049999999999999</v>
       </c>
-      <c r="W10" s="11">
+      <c r="X10" s="25">
         <v>49.394999999999996</v>
       </c>
-      <c r="X10" s="12">
+      <c r="Y10" s="24">
         <v>1.96</v>
       </c>
-      <c r="Y10" s="12">
+      <c r="Z10" s="24">
         <v>49.094999999999999</v>
       </c>
-      <c r="Z10" s="13">
+      <c r="AA10" s="26">
         <v>4</v>
       </c>
-      <c r="AA10" s="14">
+      <c r="AB10" s="27">
         <v>1.6</v>
       </c>
-      <c r="AB10" s="13">
+      <c r="AC10" s="26">
         <v>2.4</v>
       </c>
-      <c r="AC10" s="8">
+      <c r="AD10" s="28">
         <v>15.700000000000001</v>
       </c>
-      <c r="AD10" s="8">
+      <c r="AE10" s="28">
         <v>3.5999999999999996</v>
       </c>
-      <c r="AE10" s="8">
+      <c r="AF10" s="28">
         <v>12.1</v>
       </c>
-      <c r="AF10" s="4">
+      <c r="AG10" s="24">
         <v>1.6924999999999999</v>
       </c>
-      <c r="AG10" s="4">
+      <c r="AH10" s="24">
         <v>0.34999999999999964</v>
       </c>
-      <c r="AH10" s="4">
+      <c r="AI10" s="24">
         <v>0.14250000000000007</v>
       </c>
     </row>
-    <row r="11" spans="1:35">
-      <c r="A11" s="1" t="s">
+    <row r="11" spans="1:36" s="24" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A11" s="21" t="s">
         <v>23</v>
       </c>
-      <c r="B11" s="1" t="s">
+      <c r="B11" s="21" t="s">
         <v>26</v>
       </c>
-      <c r="C11" s="6">
+      <c r="C11" s="22">
         <v>3.4248148148148148</v>
       </c>
-      <c r="D11" s="6">
+      <c r="D11" s="22">
         <v>887.5</v>
       </c>
-      <c r="E11" s="4">
+      <c r="E11" s="24">
         <v>0</v>
       </c>
-      <c r="F11" s="5">
+      <c r="F11" s="23" t="s">
+        <v>55</v>
+      </c>
+      <c r="G11" s="23">
         <v>200</v>
       </c>
-      <c r="G11" s="5">
+      <c r="H11" s="23">
         <v>1.8425983760149801E-2</v>
       </c>
-      <c r="H11" s="5">
+      <c r="I11" s="23">
         <v>9.6666666666666696</v>
       </c>
-      <c r="I11" s="5">
+      <c r="J11" s="23">
         <v>27.3333333333333</v>
       </c>
-      <c r="J11" s="5">
+      <c r="K11" s="23">
         <v>37.046999999999997</v>
       </c>
-      <c r="K11" s="5">
+      <c r="L11" s="23">
         <v>17.5</v>
       </c>
-      <c r="L11" s="5">
+      <c r="M11" s="23">
         <v>-8.0278996415770703</v>
       </c>
-      <c r="M11" s="5">
+      <c r="N11" s="23">
         <v>7.2974528449820797</v>
       </c>
-      <c r="N11" s="5">
+      <c r="O11" s="23">
         <v>4.9677419354838701</v>
       </c>
-      <c r="O11" s="5">
+      <c r="P11" s="23">
         <v>149.48349999999999</v>
       </c>
-      <c r="P11" s="5">
+      <c r="Q11" s="23">
         <v>28.3675</v>
       </c>
-      <c r="Q11" s="5">
+      <c r="R11" s="23">
         <v>23.5</v>
       </c>
-      <c r="R11" s="4">
+      <c r="S11" s="24">
         <v>0.27910000000000001</v>
       </c>
-      <c r="S11" s="4">
+      <c r="T11" s="24">
         <v>3.8200000000000012E-2</v>
       </c>
-      <c r="T11" s="4">
+      <c r="U11" s="24">
         <v>0.25124999999999997</v>
       </c>
-      <c r="U11" s="4">
+      <c r="V11" s="24">
         <v>0.17065</v>
       </c>
-      <c r="V11" s="11">
+      <c r="W11" s="25">
         <v>1.83</v>
       </c>
-      <c r="W11" s="11">
+      <c r="X11" s="25">
         <v>49.09</v>
       </c>
-      <c r="X11" s="12">
+      <c r="Y11" s="24">
         <v>2.1150000000000002</v>
       </c>
-      <c r="Y11" s="12">
+      <c r="Z11" s="24">
         <v>48.475000000000001</v>
       </c>
-      <c r="Z11" s="13">
+      <c r="AA11" s="26">
         <v>6.2</v>
       </c>
-      <c r="AA11" s="14">
+      <c r="AB11" s="27">
         <v>1.2</v>
       </c>
-      <c r="AB11" s="13">
+      <c r="AC11" s="26">
         <v>5</v>
       </c>
-      <c r="AC11" s="8">
+      <c r="AD11" s="28">
         <v>10.1</v>
       </c>
-      <c r="AD11" s="8">
+      <c r="AE11" s="28">
         <v>4.3</v>
       </c>
-      <c r="AE11" s="8">
+      <c r="AF11" s="28">
         <v>5.8</v>
       </c>
-      <c r="AF11" s="4">
+      <c r="AG11" s="24">
         <v>1.0449999999999999</v>
       </c>
-      <c r="AG11" s="4">
+      <c r="AH11" s="24">
         <v>0.13250000000000028</v>
       </c>
-      <c r="AH11" s="4">
+      <c r="AI11" s="24">
         <v>0.14749999999999996</v>
       </c>
     </row>
-    <row r="12" spans="1:35">
-      <c r="A12" s="1" t="s">
+    <row r="12" spans="1:36" s="24" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A12" s="21" t="s">
         <v>24</v>
       </c>
-      <c r="B12" s="1" t="s">
+      <c r="B12" s="21" t="s">
         <v>26</v>
       </c>
-      <c r="C12" s="6">
+      <c r="C12" s="22">
         <v>1.164962962962963</v>
       </c>
-      <c r="D12" s="6">
+      <c r="D12" s="22">
         <v>1275</v>
       </c>
-      <c r="E12" s="4">
+      <c r="E12" s="24">
         <v>0</v>
       </c>
-      <c r="F12" s="5">
+      <c r="F12" s="23" t="s">
+        <v>57</v>
+      </c>
+      <c r="G12" s="23">
         <v>200</v>
       </c>
-      <c r="G12" s="5">
+      <c r="H12" s="23">
         <v>0.37173913043478302</v>
       </c>
-      <c r="H12" s="5">
+      <c r="I12" s="23">
         <v>15.633333333333301</v>
       </c>
-      <c r="I12" s="5">
+      <c r="J12" s="23">
         <v>27.3333333333333</v>
       </c>
-      <c r="J12" s="5">
+      <c r="K12" s="23">
         <v>53.361499999999999</v>
       </c>
-      <c r="K12" s="5">
+      <c r="L12" s="23">
         <v>25</v>
       </c>
-      <c r="L12" s="5">
+      <c r="M12" s="23">
         <v>-11.474756944444501</v>
       </c>
-      <c r="M12" s="5">
+      <c r="N12" s="23">
         <v>8.2591950044802793</v>
       </c>
-      <c r="N12" s="5">
+      <c r="O12" s="23">
         <v>4.4354838709677402</v>
       </c>
-      <c r="O12" s="5">
+      <c r="P12" s="23">
         <v>163.01</v>
       </c>
-      <c r="P12" s="5">
+      <c r="Q12" s="23">
         <v>96.563000000000002</v>
       </c>
-      <c r="Q12" s="5">
+      <c r="R12" s="23">
         <v>15.7</v>
       </c>
-      <c r="R12" s="4">
+      <c r="S12" s="24">
         <v>0.1961</v>
       </c>
-      <c r="S12" s="4">
+      <c r="T12" s="24">
         <v>5.6600000000000039E-2</v>
       </c>
-      <c r="T12" s="4">
+      <c r="U12" s="24">
         <v>0.22800000000000001</v>
       </c>
-      <c r="U12" s="4">
+      <c r="V12" s="24">
         <v>0.25160000000000005</v>
       </c>
-      <c r="V12" s="11">
+      <c r="W12" s="25">
         <v>1.585</v>
       </c>
-      <c r="W12" s="11">
+      <c r="X12" s="25">
         <v>49.085000000000001</v>
       </c>
-      <c r="X12" s="12">
+      <c r="Y12" s="24">
         <v>1.875</v>
       </c>
-      <c r="Y12" s="12">
+      <c r="Z12" s="24">
         <v>47.655000000000001</v>
       </c>
-      <c r="Z12" s="13">
+      <c r="AA12" s="26">
         <v>6.2</v>
       </c>
-      <c r="AA12" s="14">
+      <c r="AB12" s="27">
         <v>2</v>
       </c>
-      <c r="AB12" s="13">
+      <c r="AC12" s="26">
         <v>4.2</v>
       </c>
-      <c r="AC12" s="8">
+      <c r="AD12" s="28">
         <v>11.7</v>
       </c>
-      <c r="AD12" s="8">
+      <c r="AE12" s="28">
         <v>6.1999999999999993</v>
       </c>
-      <c r="AE12" s="8">
+      <c r="AF12" s="28">
         <v>5.5</v>
       </c>
-      <c r="AF12" s="4">
+      <c r="AG12" s="24">
         <v>1.67</v>
       </c>
-      <c r="AG12" s="4">
+      <c r="AH12" s="24">
         <v>0.39499999999999957</v>
       </c>
-      <c r="AH12" s="4">
+      <c r="AI12" s="24">
         <v>0.15249999999999986</v>
       </c>
     </row>
-    <row r="13" spans="1:35">
-      <c r="A13" s="1" t="s">
+    <row r="13" spans="1:36" s="24" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A13" s="21" t="s">
         <v>25</v>
       </c>
-      <c r="B13" s="1" t="s">
+      <c r="B13" s="21" t="s">
         <v>26</v>
       </c>
-      <c r="C13" s="6">
+      <c r="C13" s="22">
         <v>1.9496666666666667</v>
       </c>
-      <c r="D13" s="6">
+      <c r="D13" s="22">
         <v>1300</v>
       </c>
-      <c r="E13" s="4">
+      <c r="E13" s="24">
         <v>0</v>
       </c>
-      <c r="F13" s="5">
+      <c r="F13" s="24" t="s">
+        <v>51</v>
+      </c>
+      <c r="G13" s="23">
         <v>117.5</v>
       </c>
-      <c r="G13" s="5">
+      <c r="H13" s="23">
         <v>0.24942931060721399</v>
       </c>
-      <c r="H13" s="5">
+      <c r="I13" s="23">
         <v>10.766666666666699</v>
       </c>
-      <c r="I13" s="5">
+      <c r="J13" s="23">
         <v>57.6666666666667</v>
       </c>
-      <c r="J13" s="5">
+      <c r="K13" s="23">
         <v>71.8125</v>
       </c>
-      <c r="K13" s="5">
+      <c r="L13" s="23">
         <v>17.5</v>
       </c>
-      <c r="L13" s="5">
+      <c r="M13" s="23">
         <v>-12.872177979390701</v>
       </c>
-      <c r="M13" s="5">
+      <c r="N13" s="23">
         <v>9.4113959453404998</v>
       </c>
-      <c r="N13" s="5">
+      <c r="O13" s="23">
         <v>4.9838709677419404</v>
       </c>
-      <c r="O13" s="5">
+      <c r="P13" s="23">
         <v>98.531999999999996</v>
       </c>
-      <c r="P13" s="5">
+      <c r="Q13" s="23">
         <v>39.676000000000002</v>
       </c>
-      <c r="Q13" s="5">
+      <c r="R13" s="23">
         <v>13.25</v>
       </c>
-      <c r="R13" s="4">
+      <c r="S13" s="24">
         <v>0.21149999999999999</v>
       </c>
-      <c r="S13" s="4">
+      <c r="T13" s="24">
         <v>2.3199999999999998E-2</v>
       </c>
-      <c r="T13" s="4">
+      <c r="U13" s="24">
         <v>0.22839999999999999</v>
       </c>
-      <c r="U13" s="4">
+      <c r="V13" s="24">
         <v>0.16250000000000003</v>
       </c>
-      <c r="V13" s="11">
+      <c r="W13" s="25">
         <v>1.69</v>
       </c>
-      <c r="W13" s="11">
+      <c r="X13" s="25">
         <v>49.225000000000001</v>
       </c>
-      <c r="X13" s="12">
+      <c r="Y13" s="24">
         <v>2.0099999999999998</v>
       </c>
-      <c r="Y13" s="12">
+      <c r="Z13" s="24">
         <v>49.26</v>
       </c>
-      <c r="Z13" s="13">
+      <c r="AA13" s="26">
         <v>5.2</v>
       </c>
-      <c r="AA13" s="14">
+      <c r="AB13" s="27">
         <v>1.4</v>
       </c>
-      <c r="AB13" s="13">
+      <c r="AC13" s="26">
         <v>3.8</v>
       </c>
-      <c r="AC13" s="8">
+      <c r="AD13" s="28">
         <v>14.2</v>
       </c>
-      <c r="AD13" s="8">
+      <c r="AE13" s="28">
         <v>8.5</v>
       </c>
-      <c r="AE13" s="8">
+      <c r="AF13" s="28">
         <v>5.7</v>
       </c>
-      <c r="AF13" s="4">
+      <c r="AG13" s="24">
         <v>2.2075</v>
       </c>
-      <c r="AG13" s="4">
+      <c r="AH13" s="24">
         <v>0.78249999999999997</v>
       </c>
-      <c r="AH13" s="4">
+      <c r="AI13" s="24">
         <v>0.29749999999999988</v>
       </c>
     </row>
-    <row r="14" spans="1:35">
-      <c r="A14" s="1" t="s">
+    <row r="14" spans="1:36" s="24" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A14" s="21" t="s">
         <v>27</v>
       </c>
-      <c r="B14" s="1" t="s">
+      <c r="B14" s="21" t="s">
         <v>28</v>
       </c>
-      <c r="C14" s="6">
+      <c r="C14" s="22">
         <v>4.0622222222222222</v>
       </c>
-      <c r="D14" s="6">
+      <c r="D14" s="22">
         <v>652.5</v>
       </c>
-      <c r="E14" s="5">
+      <c r="E14" s="23">
         <v>37.5</v>
       </c>
-      <c r="F14" s="5">
+      <c r="F14" s="23" t="s">
+        <v>52</v>
+      </c>
+      <c r="G14" s="23">
         <v>7</v>
       </c>
-      <c r="G14" s="5">
+      <c r="H14" s="23">
         <v>0.92106979778212605</v>
       </c>
-      <c r="H14" s="5">
+      <c r="I14" s="23">
         <v>7.93333333333333</v>
       </c>
-      <c r="I14" s="5">
+      <c r="J14" s="23">
         <v>44.6666666666667</v>
       </c>
-      <c r="J14" s="5">
+      <c r="K14" s="23">
         <v>51.407499999999999</v>
       </c>
-      <c r="K14" s="5">
+      <c r="L14" s="23">
         <v>50</v>
       </c>
-      <c r="L14" s="5">
+      <c r="M14" s="23">
         <v>-4.8224193548387104</v>
       </c>
-      <c r="M14" s="5">
+      <c r="N14" s="23">
         <v>7.2897296146953403</v>
       </c>
-      <c r="N14" s="5">
+      <c r="O14" s="23">
         <v>33.290322580645203</v>
       </c>
-      <c r="O14" s="5">
+      <c r="P14" s="23">
         <v>78.292000000000002</v>
       </c>
-      <c r="P14" s="5">
+      <c r="Q14" s="23">
         <v>28.581499999999998</v>
       </c>
-      <c r="Q14" s="5">
+      <c r="R14" s="23">
         <v>20.5</v>
       </c>
-      <c r="R14" s="4">
+      <c r="S14" s="24">
         <v>0.21024999999999999</v>
       </c>
-      <c r="S14" s="4">
+      <c r="T14" s="24">
         <v>3.3800000000000024E-2</v>
       </c>
-      <c r="T14" s="4">
+      <c r="U14" s="24">
         <v>0.21565000000000001</v>
       </c>
-      <c r="U14" s="4">
+      <c r="V14" s="24">
         <v>0.21815000000000001</v>
       </c>
-      <c r="V14" s="11">
+      <c r="W14" s="25">
         <v>1.7999999999999998</v>
       </c>
-      <c r="W14" s="11">
+      <c r="X14" s="25">
         <v>49.7</v>
       </c>
-      <c r="X14" s="12">
+      <c r="Y14" s="24">
         <v>1.85</v>
       </c>
-      <c r="Y14" s="12">
+      <c r="Z14" s="24">
         <v>49.14</v>
       </c>
-      <c r="Z14" s="13">
+      <c r="AA14" s="26">
         <v>6.2</v>
       </c>
-      <c r="AA14" s="14">
+      <c r="AB14" s="27">
         <v>1.6</v>
       </c>
-      <c r="AB14" s="13">
+      <c r="AC14" s="26">
         <v>4.5999999999999996</v>
       </c>
-      <c r="AC14" s="8">
+      <c r="AD14" s="28">
         <v>14.7</v>
       </c>
-      <c r="AD14" s="8">
+      <c r="AE14" s="28">
         <v>5.7</v>
       </c>
-      <c r="AE14" s="8">
+      <c r="AF14" s="28">
         <v>9</v>
       </c>
-      <c r="AF14" s="4">
+      <c r="AG14" s="24">
         <v>2.2524999999999999</v>
       </c>
-      <c r="AG14" s="4">
+      <c r="AH14" s="24">
         <v>0.82499999999999996</v>
       </c>
-      <c r="AH14" s="4">
+      <c r="AI14" s="24">
         <v>0.27249999999999996</v>
       </c>
     </row>
-    <row r="15" spans="1:35">
-      <c r="A15" s="1" t="s">
+    <row r="15" spans="1:36" s="24" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A15" s="21" t="s">
         <v>29</v>
       </c>
-      <c r="B15" s="1" t="s">
+      <c r="B15" s="21" t="s">
         <v>28</v>
       </c>
-      <c r="C15" s="6">
+      <c r="C15" s="22">
         <v>2.1878148148148151</v>
       </c>
-      <c r="D15" s="6">
+      <c r="D15" s="22">
         <v>670</v>
       </c>
-      <c r="E15" s="5">
+      <c r="E15" s="23">
         <v>31</v>
       </c>
-      <c r="F15" s="5">
+      <c r="F15" s="24" t="s">
+        <v>51</v>
+      </c>
+      <c r="G15" s="23">
         <v>51.5</v>
       </c>
-      <c r="G15" s="5">
+      <c r="H15" s="23">
         <v>0.94950124688279303</v>
       </c>
-      <c r="H15" s="5">
+      <c r="I15" s="23">
         <v>6.3333333333333304</v>
       </c>
-      <c r="I15" s="5">
+      <c r="J15" s="23">
         <v>13.3333333333333</v>
       </c>
-      <c r="J15" s="5">
+      <c r="K15" s="23">
         <v>113.3185</v>
       </c>
-      <c r="K15" s="5">
+      <c r="L15" s="23">
         <v>25</v>
       </c>
-      <c r="L15" s="5">
+      <c r="M15" s="23">
         <v>-9.2596032706093201</v>
       </c>
-      <c r="M15" s="5">
+      <c r="N15" s="23">
         <v>8.0977513440860207</v>
       </c>
-      <c r="N15" s="5">
+      <c r="O15" s="23">
         <v>13.919354838709699</v>
       </c>
-      <c r="O15" s="5">
+      <c r="P15" s="23">
         <v>132.64150000000001</v>
       </c>
-      <c r="P15" s="5">
+      <c r="Q15" s="23">
         <v>7.0640000000000001</v>
       </c>
-      <c r="Q15" s="5">
+      <c r="R15" s="23">
         <v>11.35</v>
       </c>
-      <c r="R15" s="4">
+      <c r="S15" s="24">
         <v>0.2059</v>
       </c>
-      <c r="S15" s="4">
+      <c r="T15" s="24">
         <v>2.9850000000000015E-2</v>
       </c>
-      <c r="T15" s="4">
+      <c r="U15" s="24">
         <v>0.21665000000000001</v>
       </c>
-      <c r="U15" s="4">
+      <c r="V15" s="24">
         <v>0.1477</v>
       </c>
-      <c r="V15" s="11">
+      <c r="W15" s="25">
         <v>1.63</v>
       </c>
-      <c r="W15" s="11">
+      <c r="X15" s="25">
         <v>49.63</v>
       </c>
-      <c r="X15" s="12">
+      <c r="Y15" s="24">
         <v>1.81</v>
       </c>
-      <c r="Y15" s="12">
+      <c r="Z15" s="24">
         <v>50.055</v>
       </c>
-      <c r="Z15" s="13">
+      <c r="AA15" s="26">
         <v>10.199999999999999</v>
       </c>
-      <c r="AA15" s="14">
+      <c r="AB15" s="27">
         <v>1.6</v>
       </c>
-      <c r="AB15" s="13">
+      <c r="AC15" s="26">
         <v>8.6</v>
       </c>
-      <c r="AC15" s="8">
+      <c r="AD15" s="28">
         <v>11.7</v>
       </c>
-      <c r="AD15" s="8">
+      <c r="AE15" s="28">
         <v>4.2</v>
       </c>
-      <c r="AE15" s="8">
+      <c r="AF15" s="28">
         <v>7.5</v>
       </c>
-      <c r="AF15" s="4">
+      <c r="AG15" s="24">
         <v>2.8449999999999998</v>
       </c>
-      <c r="AG15" s="4">
+      <c r="AH15" s="24">
         <v>0.75000000000000089</v>
       </c>
-      <c r="AH15" s="4">
+      <c r="AI15" s="24">
         <v>0.21499999999999986</v>
       </c>
     </row>
-    <row r="16" spans="1:35">
-      <c r="A16" s="1" t="s">
+    <row r="16" spans="1:36" s="24" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A16" s="21" t="s">
         <v>30</v>
       </c>
-      <c r="B16" s="1" t="s">
+      <c r="B16" s="21" t="s">
         <v>28</v>
       </c>
-      <c r="C16" s="6">
+      <c r="C16" s="22">
         <v>1.7542962962962967</v>
       </c>
-      <c r="D16" s="6">
+      <c r="D16" s="22">
         <v>910</v>
       </c>
-      <c r="E16" s="5">
+      <c r="E16" s="23">
         <v>50.5</v>
       </c>
-      <c r="F16" s="5">
+      <c r="F16" s="23" t="s">
+        <v>54</v>
+      </c>
+      <c r="G16" s="23">
         <v>13.5</v>
       </c>
-      <c r="G16" s="5">
+      <c r="H16" s="23">
         <v>0.81961147086031405</v>
       </c>
-      <c r="H16" s="5">
+      <c r="I16" s="23">
         <v>7.4</v>
       </c>
-      <c r="I16" s="5">
+      <c r="J16" s="23">
         <v>84.3333333333333</v>
       </c>
-      <c r="J16" s="5">
+      <c r="K16" s="23">
         <v>61.753999999999998</v>
       </c>
-      <c r="K16" s="5">
+      <c r="L16" s="23">
         <v>37.5</v>
       </c>
-      <c r="L16" s="5">
+      <c r="M16" s="23">
         <v>-5.1680955421146901</v>
       </c>
-      <c r="M16" s="5">
+      <c r="N16" s="23">
         <v>7.1289885752688198</v>
       </c>
-      <c r="N16" s="5">
+      <c r="O16" s="23">
         <v>19.5161290322581</v>
       </c>
-      <c r="O16" s="5">
+      <c r="P16" s="23">
         <v>129.7165</v>
       </c>
-      <c r="P16" s="5">
+      <c r="Q16" s="23">
         <v>14.1195</v>
       </c>
-      <c r="Q16" s="5">
+      <c r="R16" s="23">
         <v>13.75</v>
       </c>
-      <c r="R16" s="4">
+      <c r="S16" s="24">
         <v>0.16820000000000002</v>
       </c>
-      <c r="S16" s="4">
+      <c r="T16" s="24">
         <v>6.5200000000000036E-2</v>
       </c>
-      <c r="T16" s="4">
+      <c r="U16" s="24">
         <v>0.14979999999999999</v>
       </c>
-      <c r="U16" s="4">
+      <c r="V16" s="24">
         <v>0.26680000000000004</v>
       </c>
-      <c r="V16" s="11">
+      <c r="W16" s="25">
         <v>1.6400000000000001</v>
       </c>
-      <c r="W16" s="11">
+      <c r="X16" s="25">
         <v>49.34</v>
       </c>
-      <c r="X16" s="12">
+      <c r="Y16" s="24">
         <v>1.95</v>
       </c>
-      <c r="Y16" s="12">
+      <c r="Z16" s="24">
         <v>46.33</v>
       </c>
-      <c r="Z16" s="13">
+      <c r="AA16" s="26">
         <v>4.4000000000000004</v>
       </c>
-      <c r="AA16" s="14">
+      <c r="AB16" s="27">
         <v>1.6</v>
       </c>
-      <c r="AB16" s="13">
+      <c r="AC16" s="26">
         <v>2.8</v>
       </c>
-      <c r="AC16" s="8">
+      <c r="AD16" s="28">
         <v>11.7</v>
       </c>
-      <c r="AD16" s="8">
+      <c r="AE16" s="28">
         <v>2.1</v>
       </c>
-      <c r="AE16" s="8">
+      <c r="AF16" s="28">
         <v>9.6</v>
       </c>
-      <c r="AF16" s="4">
+      <c r="AG16" s="24">
         <v>1.3725000000000001</v>
       </c>
-      <c r="AG16" s="4">
+      <c r="AH16" s="24">
         <v>0.18999999999999995</v>
       </c>
-      <c r="AH16" s="4">
+      <c r="AI16" s="24">
         <v>0.21499999999999986</v>
       </c>
     </row>
-    <row r="17" spans="1:34">
-      <c r="A17" s="1" t="s">
+    <row r="17" spans="1:35" s="24" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A17" s="21" t="s">
         <v>31</v>
       </c>
-      <c r="B17" s="1" t="s">
+      <c r="B17" s="21" t="s">
         <v>28</v>
       </c>
-      <c r="C17" s="6">
+      <c r="C17" s="22">
         <v>4.4444444444444446</v>
       </c>
-      <c r="D17" s="6">
+      <c r="D17" s="22">
         <v>955</v>
       </c>
-      <c r="E17" s="5">
+      <c r="E17" s="23">
         <v>52</v>
       </c>
-      <c r="F17" s="5">
+      <c r="F17" s="23" t="s">
+        <v>56</v>
+      </c>
+      <c r="G17" s="23">
         <v>16</v>
       </c>
-      <c r="G17" s="5">
+      <c r="H17" s="23">
         <v>0.93800667620410105</v>
       </c>
-      <c r="H17" s="5">
+      <c r="I17" s="23">
         <v>4.2</v>
       </c>
-      <c r="I17" s="5">
+      <c r="J17" s="23">
         <v>41.6666666666667</v>
       </c>
-      <c r="J17" s="5">
+      <c r="K17" s="23">
         <v>67.082499999999996</v>
       </c>
-      <c r="K17" s="5">
+      <c r="L17" s="23">
         <v>37.5</v>
       </c>
-      <c r="L17" s="5">
+      <c r="M17" s="23">
         <v>-4.52902542562724</v>
       </c>
-      <c r="M17" s="5">
+      <c r="N17" s="23">
         <v>8.3219214829749095</v>
       </c>
-      <c r="N17" s="5">
+      <c r="O17" s="23">
         <v>22.193548387096801</v>
       </c>
-      <c r="O17" s="5">
+      <c r="P17" s="23">
         <v>217.5205</v>
       </c>
-      <c r="P17" s="5">
+      <c r="Q17" s="23">
         <v>86.867500000000007</v>
       </c>
-      <c r="Q17" s="5">
+      <c r="R17" s="23">
         <v>16</v>
       </c>
-      <c r="R17" s="4">
+      <c r="S17" s="24">
         <v>0.2843</v>
       </c>
-      <c r="S17" s="4">
+      <c r="T17" s="24">
         <v>2.930000000000002E-2</v>
       </c>
-      <c r="T17" s="4">
+      <c r="U17" s="24">
         <v>0.14205000000000001</v>
       </c>
-      <c r="U17" s="4">
+      <c r="V17" s="24">
         <v>0.15615000000000001</v>
       </c>
-      <c r="V17" s="11">
+      <c r="W17" s="25">
         <v>1.9</v>
       </c>
-      <c r="W17" s="11">
+      <c r="X17" s="25">
         <v>49.204999999999998</v>
       </c>
-      <c r="X17" s="12">
+      <c r="Y17" s="24">
         <v>1.915</v>
       </c>
-      <c r="Y17" s="12">
+      <c r="Z17" s="24">
         <v>45.17</v>
       </c>
-      <c r="Z17" s="13">
+      <c r="AA17" s="26">
         <v>6.2</v>
       </c>
-      <c r="AA17" s="14">
+      <c r="AB17" s="27">
         <v>1.6</v>
       </c>
-      <c r="AB17" s="13">
+      <c r="AC17" s="26">
         <v>4.5999999999999996</v>
       </c>
-      <c r="AC17" s="8">
+      <c r="AD17" s="28">
         <v>17.55</v>
       </c>
-      <c r="AD17" s="8">
+      <c r="AE17" s="28">
         <v>12.15</v>
       </c>
-      <c r="AE17" s="8">
+      <c r="AF17" s="28">
         <v>5.4</v>
       </c>
-      <c r="AF17" s="4">
+      <c r="AG17" s="24">
         <v>1.8725000000000001</v>
       </c>
-      <c r="AG17" s="4">
+      <c r="AH17" s="24">
         <v>0.43500000000000005</v>
       </c>
-      <c r="AH17" s="4">
+      <c r="AI17" s="24">
         <v>0.23249999999999993</v>
       </c>
     </row>
-    <row r="18" spans="1:34">
-      <c r="A18" s="1" t="s">
+    <row r="18" spans="1:35" s="24" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A18" s="21" t="s">
         <v>32</v>
       </c>
-      <c r="B18" s="1" t="s">
+      <c r="B18" s="21" t="s">
         <v>28</v>
       </c>
-      <c r="C18" s="6">
+      <c r="C18" s="22">
         <v>2.3694111111111109</v>
       </c>
-      <c r="D18" s="6">
+      <c r="D18" s="22">
         <v>957.5</v>
       </c>
-      <c r="E18" s="5">
+      <c r="E18" s="23">
         <v>55.5</v>
       </c>
-      <c r="F18" s="5">
+      <c r="F18" s="23" t="s">
+        <v>51</v>
+      </c>
+      <c r="G18" s="23">
         <v>37</v>
       </c>
-      <c r="G18" s="5">
+      <c r="H18" s="23">
         <v>0.94441797681435602</v>
       </c>
-      <c r="H18" s="5">
+      <c r="I18" s="23">
         <v>7.7</v>
       </c>
-      <c r="I18" s="5">
+      <c r="J18" s="23">
         <v>45</v>
       </c>
-      <c r="J18" s="5">
+      <c r="K18" s="23">
         <v>56.587000000000003</v>
       </c>
-      <c r="K18" s="5">
+      <c r="L18" s="23">
         <v>25</v>
       </c>
-      <c r="L18" s="5">
+      <c r="M18" s="23">
         <v>-9.8810702284946306</v>
       </c>
-      <c r="M18" s="5">
+      <c r="N18" s="23">
         <v>8.1354280913978503</v>
       </c>
-      <c r="N18" s="5">
+      <c r="O18" s="23">
         <v>8.1451612903225801</v>
       </c>
-      <c r="O18" s="5">
+      <c r="P18" s="23">
         <v>195.34</v>
       </c>
-      <c r="P18" s="5">
+      <c r="Q18" s="23">
         <v>110.72799999999999</v>
       </c>
-      <c r="Q18" s="5">
+      <c r="R18" s="23">
         <v>19.75</v>
       </c>
-      <c r="R18" s="4">
+      <c r="S18" s="24">
         <v>0.23694999999999999</v>
       </c>
-      <c r="S18" s="4">
+      <c r="T18" s="24">
         <v>4.5300000000000007E-2</v>
       </c>
-      <c r="T18" s="4">
+      <c r="U18" s="24">
         <v>0.20124999999999998</v>
       </c>
-      <c r="U18" s="4">
+      <c r="V18" s="24">
         <v>8.2650000000000029E-2</v>
       </c>
-      <c r="V18" s="11">
+      <c r="W18" s="25">
         <v>1.89</v>
       </c>
-      <c r="W18" s="11">
+      <c r="X18" s="25">
         <v>49.480000000000004</v>
       </c>
-      <c r="X18" s="12">
+      <c r="Y18" s="24">
         <v>1.885</v>
       </c>
-      <c r="Y18" s="12">
+      <c r="Z18" s="24">
         <v>49.704999999999998</v>
       </c>
-      <c r="Z18" s="13">
+      <c r="AA18" s="26">
         <v>7.4</v>
       </c>
-      <c r="AA18" s="14">
+      <c r="AB18" s="27">
         <v>1.4</v>
       </c>
-      <c r="AB18" s="13">
+      <c r="AC18" s="26">
         <v>6</v>
       </c>
-      <c r="AC18" s="8">
+      <c r="AD18" s="28">
         <v>10.7</v>
       </c>
-      <c r="AD18" s="8">
+      <c r="AE18" s="28">
         <v>2.8</v>
       </c>
-      <c r="AE18" s="8">
+      <c r="AF18" s="28">
         <v>7.9</v>
       </c>
-      <c r="AF18" s="4">
+      <c r="AG18" s="24">
         <v>1.6450000000000002</v>
       </c>
-      <c r="AG18" s="4">
+      <c r="AH18" s="24">
         <v>0.14500000000000002</v>
       </c>
-      <c r="AH18" s="4">
+      <c r="AI18" s="24">
         <v>0.13000000000000034</v>
       </c>
     </row>
-    <row r="19" spans="1:34">
-      <c r="A19" s="1" t="s">
+    <row r="19" spans="1:35" s="24" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A19" s="21" t="s">
         <v>33</v>
       </c>
-      <c r="B19" s="1" t="s">
+      <c r="B19" s="21" t="s">
         <v>28</v>
       </c>
-      <c r="C19" s="6">
+      <c r="C19" s="22">
         <v>1.587777777777778</v>
       </c>
-      <c r="D19" s="6">
+      <c r="D19" s="22">
         <v>702.5</v>
       </c>
-      <c r="E19" s="5">
+      <c r="E19" s="23">
         <v>56.5</v>
       </c>
-      <c r="F19" s="5">
+      <c r="F19" s="23" t="s">
+        <v>57</v>
+      </c>
+      <c r="G19" s="23">
         <v>31.5</v>
       </c>
-      <c r="G19" s="5">
+      <c r="H19" s="23">
         <v>0.67568432847766902</v>
       </c>
-      <c r="H19" s="5">
+      <c r="I19" s="23">
         <v>9.4666666666666703</v>
       </c>
-      <c r="I19" s="5">
+      <c r="J19" s="23">
         <v>54.6666666666667</v>
       </c>
-      <c r="J19" s="5">
+      <c r="K19" s="23">
         <v>43.429000000000002</v>
       </c>
-      <c r="K19" s="5">
+      <c r="L19" s="23">
         <v>50</v>
       </c>
-      <c r="L19" s="5">
+      <c r="M19" s="23">
         <v>-7.45969545250896</v>
       </c>
-      <c r="M19" s="5">
+      <c r="N19" s="23">
         <v>6.1849107302867399</v>
       </c>
-      <c r="N19" s="5">
+      <c r="O19" s="23">
         <v>17.645161290322601</v>
       </c>
-      <c r="O19" s="5">
+      <c r="P19" s="23">
         <v>120.9205</v>
       </c>
-      <c r="P19" s="5">
+      <c r="Q19" s="23">
         <v>47.137500000000003</v>
       </c>
-      <c r="Q19" s="5">
+      <c r="R19" s="23">
         <v>29.7</v>
       </c>
-      <c r="R19" s="4">
+      <c r="S19" s="24">
         <v>0.24829999999999999</v>
       </c>
-      <c r="S19" s="4">
+      <c r="T19" s="24">
         <v>4.5499999999999985E-2</v>
       </c>
-      <c r="T19" s="4">
+      <c r="U19" s="24">
         <v>0.23799999999999999</v>
       </c>
-      <c r="U19" s="4">
+      <c r="V19" s="24">
         <v>0.17810000000000004</v>
       </c>
-      <c r="V19" s="11">
+      <c r="W19" s="25">
         <v>2.11</v>
       </c>
-      <c r="W19" s="11">
+      <c r="X19" s="25">
         <v>49.71</v>
       </c>
-      <c r="X19" s="12">
+      <c r="Y19" s="24">
         <v>1.79</v>
       </c>
-      <c r="Y19" s="12">
+      <c r="Z19" s="24">
         <v>48.74</v>
       </c>
-      <c r="Z19" s="13">
+      <c r="AA19" s="26">
         <v>14.4</v>
       </c>
-      <c r="AA19" s="14">
+      <c r="AB19" s="27">
         <v>1.6</v>
       </c>
-      <c r="AB19" s="13">
+      <c r="AC19" s="26">
         <v>12.8</v>
       </c>
-      <c r="AC19" s="8">
+      <c r="AD19" s="28">
         <v>8.6999999999999993</v>
       </c>
-      <c r="AD19" s="8">
+      <c r="AE19" s="28">
         <v>3.0999999999999996</v>
       </c>
-      <c r="AE19" s="8">
+      <c r="AF19" s="28">
         <v>5.6</v>
       </c>
-      <c r="AF19" s="4">
+      <c r="AG19" s="24">
         <v>1.7074999999999998</v>
       </c>
-      <c r="AG19" s="4">
+      <c r="AH19" s="24">
         <v>0.1875</v>
       </c>
-      <c r="AH19" s="4">
+      <c r="AI19" s="24">
         <v>0.32749999999999968</v>
       </c>
     </row>
-    <row r="20" spans="1:34">
-      <c r="A20" s="1" t="s">
+    <row r="20" spans="1:35" s="24" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A20" s="21" t="s">
         <v>27</v>
       </c>
-      <c r="B20" s="1" t="s">
+      <c r="B20" s="21" t="s">
         <v>34</v>
       </c>
-      <c r="C20" s="6">
+      <c r="C20" s="22">
         <v>2.5792222222222225</v>
       </c>
-      <c r="D20" s="6">
+      <c r="D20" s="22">
         <v>1575</v>
       </c>
-      <c r="E20" s="4">
+      <c r="E20" s="24">
         <v>0</v>
       </c>
-      <c r="F20" s="5">
+      <c r="F20" s="23" t="s">
+        <v>52</v>
+      </c>
+      <c r="G20" s="23">
         <v>112.5</v>
       </c>
-      <c r="G20" s="5">
+      <c r="H20" s="23">
         <v>4.2418772563176901E-2</v>
       </c>
-      <c r="H20" s="5">
+      <c r="I20" s="23">
         <v>13.633333333333301</v>
       </c>
-      <c r="I20" s="5">
+      <c r="J20" s="23">
         <v>52</v>
       </c>
-      <c r="J20" s="5">
+      <c r="K20" s="23">
         <v>68.245500000000007</v>
       </c>
-      <c r="K20" s="5">
+      <c r="L20" s="23">
         <v>37.5</v>
       </c>
-      <c r="L20" s="5">
+      <c r="M20" s="23">
         <v>-8.3393536066308194</v>
       </c>
-      <c r="M20" s="5">
+      <c r="N20" s="23">
         <v>10.4188732078853</v>
       </c>
-      <c r="N20" s="5">
+      <c r="O20" s="23">
         <v>16.612903225806502</v>
       </c>
-      <c r="O20" s="5">
+      <c r="P20" s="23">
         <v>30.609000000000002</v>
       </c>
-      <c r="P20" s="5">
+      <c r="Q20" s="23">
         <v>3.2813620959945702</v>
       </c>
-      <c r="Q20" s="5">
+      <c r="R20" s="23">
         <v>12.25</v>
       </c>
-      <c r="R20" s="4">
+      <c r="S20" s="24">
         <v>0.31735000000000002</v>
       </c>
-      <c r="S20" s="4">
+      <c r="T20" s="24">
         <v>2.3900000000000032E-2</v>
       </c>
-      <c r="T20" s="4">
+      <c r="U20" s="24">
         <v>0.17369999999999999</v>
       </c>
-      <c r="U20" s="4">
+      <c r="V20" s="24">
         <v>0.27539999999999998</v>
       </c>
-      <c r="V20" s="11">
+      <c r="W20" s="25">
         <v>1.79</v>
       </c>
-      <c r="W20" s="11">
+      <c r="X20" s="25">
         <v>49.204999999999998</v>
       </c>
-      <c r="X20" s="12">
+      <c r="Y20" s="24">
         <v>2.25</v>
       </c>
-      <c r="Y20" s="12">
+      <c r="Z20" s="24">
         <v>47.55</v>
       </c>
-      <c r="Z20" s="13">
+      <c r="AA20" s="26">
         <v>25.6</v>
       </c>
-      <c r="AA20" s="14">
+      <c r="AB20" s="27">
         <v>1.6</v>
       </c>
-      <c r="AB20" s="13">
+      <c r="AC20" s="26">
         <v>24</v>
       </c>
-      <c r="AC20" s="8">
+      <c r="AD20" s="28">
         <v>21.9</v>
       </c>
-      <c r="AD20" s="8">
+      <c r="AE20" s="28">
         <v>5.0999999999999996</v>
       </c>
-      <c r="AE20" s="8">
+      <c r="AF20" s="28">
         <v>16.8</v>
       </c>
-      <c r="AF20" s="4">
+      <c r="AG20" s="24">
         <v>2.4575</v>
       </c>
-      <c r="AG20" s="4">
+      <c r="AH20" s="24">
         <v>0.36749999999999972</v>
       </c>
-      <c r="AH20" s="4">
+      <c r="AI20" s="24">
         <v>0.30500000000000016</v>
       </c>
     </row>
-    <row r="21" spans="1:34">
-      <c r="A21" s="1" t="s">
+    <row r="21" spans="1:35" s="24" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A21" s="21" t="s">
         <v>29</v>
       </c>
-      <c r="B21" s="1" t="s">
+      <c r="B21" s="21" t="s">
         <v>34</v>
       </c>
-      <c r="C21" s="6">
+      <c r="C21" s="22">
         <v>1.3692222222222219</v>
       </c>
-      <c r="D21" s="6">
+      <c r="D21" s="22">
         <v>797.5</v>
       </c>
-      <c r="E21" s="4">
+      <c r="E21" s="24">
         <v>0</v>
       </c>
-      <c r="F21" s="5">
+      <c r="F21" s="24" t="s">
+        <v>51</v>
+      </c>
+      <c r="G21" s="23">
         <v>116.5</v>
       </c>
-      <c r="G21" s="5">
+      <c r="H21" s="23">
         <v>0</v>
       </c>
-      <c r="H21" s="5">
+      <c r="I21" s="23">
         <v>7.6333333333333302</v>
       </c>
-      <c r="I21" s="5">
+      <c r="J21" s="23">
         <v>42.6666666666667</v>
       </c>
-      <c r="J21" s="5">
+      <c r="K21" s="23">
         <v>93.576499999999996</v>
       </c>
-      <c r="K21" s="5">
+      <c r="L21" s="23">
         <v>25</v>
       </c>
-      <c r="L21" s="5">
+      <c r="M21" s="23">
         <v>-6.1423118279569904</v>
       </c>
-      <c r="M21" s="5">
+      <c r="N21" s="23">
         <v>8.0615549955197103</v>
       </c>
-      <c r="N21" s="5">
+      <c r="O21" s="23">
         <v>14.919354838709699</v>
       </c>
-      <c r="O21" s="5">
+      <c r="P21" s="23">
         <v>44.756</v>
       </c>
-      <c r="P21" s="5">
+      <c r="Q21" s="23">
         <v>17.158000000000001</v>
       </c>
-      <c r="Q21" s="5">
+      <c r="R21" s="23">
         <v>9</v>
       </c>
-      <c r="R21" s="4">
+      <c r="S21" s="24">
         <v>0.21990000000000001</v>
       </c>
-      <c r="S21" s="4">
+      <c r="T21" s="24">
         <v>2.2300000000000014E-2</v>
       </c>
-      <c r="T21" s="4">
+      <c r="U21" s="24">
         <v>0.22675000000000001</v>
       </c>
-      <c r="U21" s="4">
+      <c r="V21" s="24">
         <v>0.12355000000000002</v>
       </c>
-      <c r="V21" s="11">
+      <c r="W21" s="25">
         <v>1.91</v>
       </c>
-      <c r="W21" s="11">
+      <c r="X21" s="25">
         <v>49.344999999999999</v>
       </c>
-      <c r="X21" s="12">
+      <c r="Y21" s="24">
         <v>2.1100000000000003</v>
       </c>
-      <c r="Y21" s="12">
+      <c r="Z21" s="24">
         <v>48.59</v>
       </c>
-      <c r="Z21" s="13">
+      <c r="AA21" s="26">
         <v>5.8</v>
       </c>
-      <c r="AA21" s="14">
+      <c r="AB21" s="27">
         <v>1.6</v>
       </c>
-      <c r="AB21" s="13">
+      <c r="AC21" s="26">
         <v>4.2</v>
       </c>
-      <c r="AC21" s="8">
+      <c r="AD21" s="28">
         <v>13.4</v>
       </c>
-      <c r="AD21" s="8">
+      <c r="AE21" s="28">
         <v>5.3999999999999995</v>
       </c>
-      <c r="AE21" s="8">
+      <c r="AF21" s="28">
         <v>8</v>
       </c>
-      <c r="AF21" s="4">
+      <c r="AG21" s="24">
         <v>1.5150000000000001</v>
       </c>
-      <c r="AG21" s="4">
+      <c r="AH21" s="24">
         <v>0.34999999999999964</v>
       </c>
-      <c r="AH21" s="4">
+      <c r="AI21" s="24">
         <v>0.53500000000000014</v>
       </c>
     </row>
-    <row r="22" spans="1:34">
-      <c r="A22" s="1" t="s">
+    <row r="22" spans="1:35" s="24" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A22" s="21" t="s">
         <v>30</v>
       </c>
-      <c r="B22" s="1" t="s">
+      <c r="B22" s="21" t="s">
         <v>34</v>
       </c>
-      <c r="C22" s="6">
+      <c r="C22" s="22">
         <v>3.1662592592592591</v>
       </c>
-      <c r="D22" s="6">
+      <c r="D22" s="22">
         <v>927.5</v>
       </c>
-      <c r="E22" s="4">
+      <c r="E22" s="24">
         <v>0</v>
       </c>
-      <c r="F22" s="5">
+      <c r="F22" s="23" t="s">
+        <v>54</v>
+      </c>
+      <c r="G22" s="23">
         <v>137.5</v>
       </c>
-      <c r="G22" s="5">
+      <c r="H22" s="23">
         <v>0</v>
       </c>
-      <c r="H22" s="5">
+      <c r="I22" s="23">
         <v>5.6666666666666696</v>
       </c>
-      <c r="I22" s="5">
+      <c r="J22" s="23">
         <v>11.3333333333333</v>
       </c>
-      <c r="J22" s="5">
+      <c r="K22" s="23">
         <v>51.012999999999998</v>
       </c>
-      <c r="K22" s="5">
+      <c r="L22" s="23">
         <v>50</v>
       </c>
-      <c r="L22" s="5">
+      <c r="M22" s="23">
         <v>-12.3296378808244</v>
       </c>
-      <c r="M22" s="5">
+      <c r="N22" s="23">
         <v>10.642083781362</v>
       </c>
-      <c r="N22" s="5">
+      <c r="O22" s="23">
         <v>25.887096774193498</v>
       </c>
-      <c r="O22" s="5">
+      <c r="P22" s="23">
         <v>148.2595</v>
       </c>
-      <c r="P22" s="5">
+      <c r="Q22" s="23">
         <v>15.035</v>
       </c>
-      <c r="Q22" s="5">
+      <c r="R22" s="23">
         <v>25.45</v>
       </c>
-      <c r="R22" s="4">
+      <c r="S22" s="24">
         <v>0.19465000000000002</v>
       </c>
-      <c r="S22" s="4">
+      <c r="T22" s="24">
         <v>4.7900000000000026E-2</v>
       </c>
-      <c r="T22" s="4">
+      <c r="U22" s="24">
         <v>0.19295000000000001</v>
       </c>
-      <c r="U22" s="4">
+      <c r="V22" s="24">
         <v>0.18735000000000002</v>
       </c>
-      <c r="V22" s="11">
+      <c r="W22" s="25">
         <v>1.835</v>
       </c>
-      <c r="W22" s="11">
+      <c r="X22" s="25">
         <v>49.594999999999999</v>
       </c>
-      <c r="X22" s="12">
+      <c r="Y22" s="24">
         <v>1.94</v>
       </c>
-      <c r="Y22" s="12">
+      <c r="Z22" s="24">
         <v>49.045000000000002</v>
       </c>
-      <c r="Z22" s="13">
+      <c r="AA22" s="26">
         <v>21.8</v>
       </c>
-      <c r="AA22" s="14">
+      <c r="AB22" s="27">
         <v>0.6</v>
       </c>
-      <c r="AB22" s="13">
+      <c r="AC22" s="26">
         <v>21.2</v>
       </c>
-      <c r="AC22" s="8">
+      <c r="AD22" s="28">
         <v>29.700000000000003</v>
       </c>
-      <c r="AD22" s="8">
+      <c r="AE22" s="28">
         <v>8.9</v>
       </c>
-      <c r="AE22" s="8">
+      <c r="AF22" s="28">
         <v>20.8</v>
       </c>
-      <c r="AF22" s="4">
+      <c r="AG22" s="24">
         <v>1.5700000000000003</v>
       </c>
-      <c r="AG22" s="4">
+      <c r="AH22" s="24">
         <v>0.24500000000000011</v>
       </c>
-      <c r="AH22" s="4">
+      <c r="AI22" s="24">
         <v>0.14749999999999996</v>
       </c>
     </row>
-    <row r="23" spans="1:34">
-      <c r="A23" s="1" t="s">
+    <row r="23" spans="1:35" s="24" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A23" s="21" t="s">
         <v>31</v>
       </c>
-      <c r="B23" s="1" t="s">
+      <c r="B23" s="21" t="s">
         <v>34</v>
       </c>
-      <c r="C23" s="6">
+      <c r="C23" s="22">
         <v>4.41</v>
       </c>
-      <c r="D23" s="6">
+      <c r="D23" s="22">
         <v>1475</v>
       </c>
-      <c r="E23" s="4">
+      <c r="E23" s="24">
         <v>0</v>
       </c>
-      <c r="F23" s="5">
+      <c r="F23" s="23" t="s">
+        <v>56</v>
+      </c>
+      <c r="G23" s="23">
         <v>108</v>
       </c>
-      <c r="G23" s="5">
+      <c r="H23" s="23">
         <v>0.148267008985879</v>
       </c>
-      <c r="H23" s="5">
+      <c r="I23" s="23">
         <v>7.0333333333333297</v>
       </c>
-      <c r="I23" s="5">
+      <c r="J23" s="23">
         <v>20.3333333333333</v>
       </c>
-      <c r="J23" s="5">
+      <c r="K23" s="23">
         <v>84.822500000000005</v>
       </c>
-      <c r="K23" s="5">
+      <c r="L23" s="23">
         <v>17.5</v>
       </c>
-      <c r="L23" s="5">
+      <c r="M23" s="23">
         <v>-10.648525985663101</v>
       </c>
-      <c r="M23" s="5">
+      <c r="N23" s="23">
         <v>11.3220650761649</v>
       </c>
-      <c r="N23" s="5">
+      <c r="O23" s="23">
         <v>7.4516129032258096</v>
       </c>
-      <c r="O23" s="5">
+      <c r="P23" s="23">
         <v>65.441000000000003</v>
       </c>
-      <c r="P23" s="5">
+      <c r="Q23" s="23">
         <v>31.102499999999999</v>
       </c>
-      <c r="Q23" s="5">
+      <c r="R23" s="23">
         <v>12.625</v>
       </c>
-      <c r="R23" s="4">
+      <c r="S23" s="24">
         <v>0.22295000000000001</v>
       </c>
-      <c r="S23" s="4">
+      <c r="T23" s="24">
         <v>0.1356</v>
       </c>
-      <c r="T23" s="4">
+      <c r="U23" s="24">
         <v>0.26780000000000004</v>
       </c>
-      <c r="U23" s="4">
+      <c r="V23" s="24">
         <v>0.1328</v>
       </c>
-      <c r="V23" s="11">
+      <c r="W23" s="25">
         <v>1.93</v>
       </c>
-      <c r="W23" s="11">
+      <c r="X23" s="25">
         <v>49.07</v>
       </c>
-      <c r="X23" s="12">
+      <c r="Y23" s="24">
         <v>2.0150000000000001</v>
       </c>
-      <c r="Y23" s="12">
+      <c r="Z23" s="24">
         <v>49.234999999999999</v>
       </c>
-      <c r="Z23" s="13">
+      <c r="AA23" s="26">
         <v>8.8000000000000007</v>
       </c>
-      <c r="AA23" s="14">
+      <c r="AB23" s="27">
         <v>1</v>
       </c>
-      <c r="AB23" s="13">
+      <c r="AC23" s="26">
         <v>7.8</v>
       </c>
-      <c r="AC23" s="8">
+      <c r="AD23" s="28">
         <v>17</v>
       </c>
-      <c r="AD23" s="8">
+      <c r="AE23" s="28">
         <v>8.6999999999999993</v>
       </c>
-      <c r="AE23" s="8">
+      <c r="AF23" s="28">
         <v>8.3000000000000007</v>
       </c>
-      <c r="AF23" s="4">
+      <c r="AG23" s="24">
         <v>2.5049999999999999</v>
       </c>
-      <c r="AG23" s="4">
+      <c r="AH23" s="24">
         <v>0.96</v>
       </c>
-      <c r="AH23" s="4">
+      <c r="AI23" s="24">
         <v>0.24500000000000099</v>
       </c>
     </row>
-    <row r="24" spans="1:34">
-      <c r="A24" s="1" t="s">
+    <row r="24" spans="1:35" s="24" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A24" s="21" t="s">
         <v>32</v>
       </c>
-      <c r="B24" s="1" t="s">
+      <c r="B24" s="21" t="s">
         <v>34</v>
       </c>
-      <c r="C24" s="6">
+      <c r="C24" s="22">
         <v>1.5285555555555554</v>
       </c>
-      <c r="D24" s="6">
+      <c r="D24" s="22">
         <v>1450</v>
       </c>
-      <c r="E24" s="4">
+      <c r="E24" s="24">
         <v>0</v>
       </c>
-      <c r="F24" s="5">
+      <c r="F24" s="24" t="s">
+        <v>51</v>
+      </c>
+      <c r="G24" s="23">
         <v>200</v>
       </c>
-      <c r="G24" s="5">
+      <c r="H24" s="23">
         <v>0.152712449043587</v>
       </c>
-      <c r="H24" s="5">
+      <c r="I24" s="23">
         <v>26.1666666666667</v>
       </c>
-      <c r="I24" s="5">
+      <c r="J24" s="23">
         <v>8</v>
       </c>
-      <c r="J24" s="5">
+      <c r="K24" s="23">
         <v>73.284000000000006</v>
       </c>
-      <c r="K24" s="5">
+      <c r="L24" s="23">
         <v>25</v>
       </c>
-      <c r="L24" s="5">
+      <c r="M24" s="23">
         <v>-9.4584460125447993</v>
       </c>
-      <c r="M24" s="5">
+      <c r="N24" s="23">
         <v>8.9011477374551902</v>
       </c>
-      <c r="N24" s="5">
+      <c r="O24" s="23">
         <v>10.0161290322581</v>
       </c>
-      <c r="O24" s="5">
+      <c r="P24" s="23">
         <v>104.70399999999999</v>
       </c>
-      <c r="P24" s="5">
+      <c r="Q24" s="23">
         <v>90.855000000000004</v>
       </c>
-      <c r="Q24" s="5">
+      <c r="R24" s="23">
         <v>17.100000000000001</v>
       </c>
-      <c r="R24" s="4">
+      <c r="S24" s="24">
         <v>0.18709999999999999</v>
       </c>
-      <c r="S24" s="4">
+      <c r="T24" s="24">
         <v>4.6999999999999986E-2</v>
       </c>
-      <c r="T24" s="4">
+      <c r="U24" s="24">
         <v>0.25839999999999996</v>
       </c>
-      <c r="U24" s="4">
+      <c r="V24" s="24">
         <v>0.14760000000000001</v>
       </c>
-      <c r="V24" s="11">
+      <c r="W24" s="25">
         <v>1.645</v>
       </c>
-      <c r="W24" s="11">
+      <c r="X24" s="25">
         <v>49.204999999999998</v>
       </c>
-      <c r="X24" s="12">
+      <c r="Y24" s="24">
         <v>1.91</v>
       </c>
-      <c r="Y24" s="12">
+      <c r="Z24" s="24">
         <v>49.814999999999998</v>
       </c>
-      <c r="Z24" s="13">
+      <c r="AA24" s="26">
         <v>5</v>
       </c>
-      <c r="AA24" s="14">
+      <c r="AB24" s="27">
         <v>1.6</v>
       </c>
-      <c r="AB24" s="13">
+      <c r="AC24" s="26">
         <v>3.4</v>
       </c>
-      <c r="AC24" s="8">
+      <c r="AD24" s="28">
         <v>11.8</v>
       </c>
-      <c r="AD24" s="8">
+      <c r="AE24" s="28">
         <v>6.3000000000000007</v>
       </c>
-      <c r="AE24" s="8">
+      <c r="AF24" s="28">
         <v>5.5</v>
       </c>
-      <c r="AF24" s="4">
+      <c r="AG24" s="24">
         <v>1.6149999999999998</v>
       </c>
-      <c r="AG24" s="4">
+      <c r="AH24" s="24">
         <v>0.33999999999999986</v>
       </c>
-      <c r="AH24" s="4">
+      <c r="AI24" s="24">
         <v>0.19249999999999989</v>
       </c>
     </row>
-    <row r="25" spans="1:34">
-      <c r="A25" s="1" t="s">
+    <row r="25" spans="1:35" s="24" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A25" s="21" t="s">
         <v>33</v>
       </c>
-      <c r="B25" s="1" t="s">
+      <c r="B25" s="21" t="s">
         <v>34</v>
       </c>
-      <c r="C25" s="6">
+      <c r="C25" s="22">
         <v>3.0546666666666664</v>
       </c>
-      <c r="D25" s="6">
+      <c r="D25" s="22">
         <v>1455</v>
       </c>
-      <c r="E25" s="4">
+      <c r="E25" s="24">
         <v>0</v>
       </c>
-      <c r="F25" s="5">
+      <c r="F25" s="23" t="s">
+        <v>57</v>
+      </c>
+      <c r="G25" s="23">
         <v>113.5</v>
       </c>
-      <c r="G25" s="5">
+      <c r="H25" s="23">
         <v>0.137077196957436</v>
       </c>
-      <c r="H25" s="5">
+      <c r="I25" s="23">
         <v>19.533333333333299</v>
       </c>
-      <c r="I25" s="5">
+      <c r="J25" s="23">
         <v>8.3333333333333304</v>
       </c>
-      <c r="J25" s="5">
+      <c r="K25" s="23">
         <v>86.259</v>
       </c>
-      <c r="K25" s="5">
+      <c r="L25" s="23">
         <v>25</v>
       </c>
-      <c r="L25" s="5">
+      <c r="M25" s="23">
         <v>-10.261255376344099</v>
       </c>
-      <c r="M25" s="5">
+      <c r="N25" s="23">
         <v>10.569398969534101</v>
       </c>
-      <c r="N25" s="5">
+      <c r="O25" s="23">
         <v>11.9032258064516</v>
       </c>
-      <c r="O25" s="5">
+      <c r="P25" s="23">
         <v>123.654</v>
       </c>
-      <c r="P25" s="5">
+      <c r="Q25" s="23">
         <v>68.242999999999995</v>
       </c>
-      <c r="Q25" s="5">
+      <c r="R25" s="23">
         <v>28.25</v>
       </c>
-      <c r="R25" s="4">
+      <c r="S25" s="24">
         <v>0.23699999999999999</v>
       </c>
-      <c r="S25" s="4">
+      <c r="T25" s="24">
         <v>5.5400000000000005E-2</v>
       </c>
-      <c r="T25" s="4">
+      <c r="U25" s="24">
         <v>0.27729999999999999</v>
       </c>
-      <c r="U25" s="4">
+      <c r="V25" s="24">
         <v>0.27154999999999996</v>
       </c>
-      <c r="V25" s="11">
+      <c r="W25" s="25">
         <v>1.8149999999999999</v>
       </c>
-      <c r="W25" s="11">
+      <c r="X25" s="25">
         <v>50.094999999999999</v>
       </c>
-      <c r="X25" s="12">
+      <c r="Y25" s="24">
         <v>2.0549999999999997</v>
       </c>
-      <c r="Y25" s="12">
+      <c r="Z25" s="24">
         <v>48.445</v>
       </c>
-      <c r="Z25" s="13">
+      <c r="AA25" s="26">
         <v>17.600000000000001</v>
       </c>
-      <c r="AA25" s="14">
+      <c r="AB25" s="27">
         <v>13</v>
       </c>
-      <c r="AB25" s="13">
+      <c r="AC25" s="26">
         <v>4.5999999999999996</v>
       </c>
-      <c r="AC25" s="8">
+      <c r="AD25" s="28">
         <v>31.5</v>
       </c>
-      <c r="AD25" s="8">
+      <c r="AE25" s="28">
         <v>25.8</v>
       </c>
-      <c r="AE25" s="8">
+      <c r="AF25" s="28">
         <v>5.7</v>
       </c>
-      <c r="AF25" s="4">
+      <c r="AG25" s="24">
         <v>2.2400000000000002</v>
       </c>
-      <c r="AG25" s="4">
+      <c r="AH25" s="24">
         <v>1.0400000000000005</v>
       </c>
-      <c r="AH25" s="4">
+      <c r="AI25" s="24">
         <v>0.20750000000000002</v>
       </c>
-    </row>
-    <row r="26" spans="1:34">
-      <c r="V26" s="12"/>
-      <c r="W26" s="12"/>
-    </row>
-    <row r="27" spans="1:34">
-      <c r="V27" s="12"/>
-      <c r="W27" s="12"/>
-    </row>
-    <row r="28" spans="1:34">
-      <c r="V28" s="12"/>
-      <c r="W28" s="12"/>
-    </row>
-    <row r="29" spans="1:34">
-      <c r="V29" s="12"/>
-      <c r="W29" s="12"/>
-    </row>
-    <row r="30" spans="1:34">
-      <c r="V30" s="12"/>
-      <c r="W30" s="12"/>
-    </row>
-    <row r="31" spans="1:34">
-      <c r="V31" s="12"/>
-      <c r="W31" s="12"/>
-    </row>
-    <row r="32" spans="1:34">
-      <c r="V32" s="12"/>
-      <c r="W32" s="12"/>
-    </row>
-    <row r="33" spans="22:23">
-      <c r="V33" s="12"/>
-      <c r="W33" s="12"/>
-    </row>
-    <row r="34" spans="22:23">
-      <c r="V34" s="12"/>
-      <c r="W34" s="12"/>
-    </row>
-    <row r="35" spans="22:23">
-      <c r="V35" s="12"/>
-      <c r="W35" s="12"/>
-    </row>
-    <row r="36" spans="22:23">
-      <c r="V36" s="12"/>
-      <c r="W36" s="12"/>
-    </row>
-    <row r="37" spans="22:23">
-      <c r="V37" s="12"/>
-      <c r="W37" s="12"/>
-    </row>
-    <row r="38" spans="22:23">
-      <c r="V38" s="12"/>
-      <c r="W38" s="12"/>
-    </row>
-    <row r="39" spans="22:23">
-      <c r="V39" s="12"/>
-      <c r="W39" s="12"/>
-    </row>
-    <row r="40" spans="22:23">
-      <c r="V40" s="12"/>
-      <c r="W40" s="12"/>
-    </row>
-    <row r="41" spans="22:23">
-      <c r="V41" s="12"/>
-      <c r="W41" s="12"/>
-    </row>
-    <row r="42" spans="22:23">
-      <c r="V42" s="12"/>
-      <c r="W42" s="12"/>
-    </row>
-    <row r="43" spans="22:23">
-      <c r="V43" s="12"/>
-      <c r="W43" s="12"/>
-    </row>
-    <row r="44" spans="22:23">
-      <c r="V44" s="12"/>
-      <c r="W44" s="12"/>
-    </row>
-    <row r="45" spans="22:23">
-      <c r="V45" s="12"/>
-      <c r="W45" s="12"/>
-    </row>
-    <row r="46" spans="22:23">
-      <c r="V46" s="12"/>
-      <c r="W46" s="12"/>
-    </row>
-    <row r="47" spans="22:23">
-      <c r="V47" s="12"/>
-      <c r="W47" s="12"/>
-    </row>
-    <row r="48" spans="22:23">
-      <c r="V48" s="12"/>
-      <c r="W48" s="12"/>
-    </row>
-    <row r="49" spans="22:23">
-      <c r="V49" s="12"/>
-      <c r="W49" s="12"/>
-    </row>
-    <row r="50" spans="22:23">
-      <c r="V50" s="12"/>
-      <c r="W50" s="12"/>
-    </row>
-    <row r="51" spans="22:23">
-      <c r="V51" s="12"/>
-      <c r="W51" s="12"/>
-    </row>
-    <row r="52" spans="22:23">
-      <c r="V52" s="12"/>
-      <c r="W52" s="12"/>
-    </row>
-    <row r="53" spans="22:23">
-      <c r="V53" s="12"/>
-      <c r="W53" s="12"/>
-    </row>
-    <row r="54" spans="22:23">
-      <c r="V54" s="12"/>
-      <c r="W54" s="12"/>
-    </row>
-    <row r="55" spans="22:23">
-      <c r="V55" s="12"/>
-      <c r="W55" s="12"/>
-    </row>
-    <row r="56" spans="22:23">
-      <c r="V56" s="12"/>
-      <c r="W56" s="12"/>
-    </row>
-    <row r="57" spans="22:23">
-      <c r="V57" s="12"/>
-      <c r="W57" s="12"/>
-    </row>
-    <row r="58" spans="22:23">
-      <c r="V58" s="12"/>
-      <c r="W58" s="12"/>
-    </row>
-    <row r="59" spans="22:23">
-      <c r="V59" s="12"/>
-      <c r="W59" s="12"/>
-    </row>
-    <row r="60" spans="22:23">
-      <c r="V60" s="12"/>
-      <c r="W60" s="12"/>
-    </row>
-    <row r="61" spans="22:23">
-      <c r="V61" s="12"/>
-      <c r="W61" s="12"/>
-    </row>
-    <row r="62" spans="22:23">
-      <c r="V62" s="12"/>
-      <c r="W62" s="12"/>
-    </row>
-    <row r="63" spans="22:23">
-      <c r="V63" s="12"/>
-      <c r="W63" s="12"/>
-    </row>
-    <row r="64" spans="22:23">
-      <c r="V64" s="12"/>
-      <c r="W64" s="12"/>
-    </row>
-    <row r="65" spans="22:23">
-      <c r="V65" s="12"/>
-      <c r="W65" s="12"/>
-    </row>
-    <row r="66" spans="22:23">
-      <c r="V66" s="12"/>
-      <c r="W66" s="12"/>
-    </row>
-    <row r="67" spans="22:23">
-      <c r="V67" s="12"/>
-      <c r="W67" s="12"/>
-    </row>
-    <row r="68" spans="22:23">
-      <c r="V68" s="12"/>
-      <c r="W68" s="12"/>
-    </row>
-    <row r="69" spans="22:23">
-      <c r="V69" s="12"/>
-      <c r="W69" s="12"/>
-    </row>
-    <row r="70" spans="22:23">
-      <c r="V70" s="12"/>
-      <c r="W70" s="12"/>
-    </row>
-    <row r="71" spans="22:23">
-      <c r="V71" s="12"/>
-      <c r="W71" s="12"/>
-    </row>
-    <row r="72" spans="22:23">
-      <c r="V72" s="12"/>
-      <c r="W72" s="12"/>
-    </row>
-    <row r="73" spans="22:23">
-      <c r="V73" s="12"/>
-      <c r="W73" s="12"/>
-    </row>
-    <row r="74" spans="22:23">
-      <c r="V74" s="12"/>
-      <c r="W74" s="12"/>
-    </row>
-    <row r="75" spans="22:23">
-      <c r="V75" s="12"/>
-      <c r="W75" s="12"/>
-    </row>
-    <row r="76" spans="22:23">
-      <c r="V76" s="12"/>
-      <c r="W76" s="12"/>
-    </row>
-    <row r="77" spans="22:23">
-      <c r="V77" s="12"/>
-      <c r="W77" s="12"/>
-    </row>
-    <row r="78" spans="22:23">
-      <c r="V78" s="12"/>
-      <c r="W78" s="12"/>
-    </row>
-    <row r="79" spans="22:23">
-      <c r="V79" s="12"/>
-      <c r="W79" s="12"/>
-    </row>
-    <row r="80" spans="22:23">
-      <c r="V80" s="12"/>
-      <c r="W80" s="12"/>
-    </row>
-    <row r="81" spans="22:23">
-      <c r="V81" s="12"/>
-      <c r="W81" s="12"/>
-    </row>
-    <row r="82" spans="22:23">
-      <c r="V82" s="12"/>
-      <c r="W82" s="12"/>
-    </row>
-    <row r="83" spans="22:23">
-      <c r="V83" s="12"/>
-      <c r="W83" s="12"/>
-    </row>
-    <row r="84" spans="22:23">
-      <c r="V84" s="12"/>
-      <c r="W84" s="12"/>
-    </row>
-    <row r="85" spans="22:23">
-      <c r="V85" s="12"/>
-      <c r="W85" s="12"/>
-    </row>
-    <row r="86" spans="22:23">
-      <c r="V86" s="12"/>
-      <c r="W86" s="12"/>
-    </row>
-    <row r="87" spans="22:23">
-      <c r="V87" s="12"/>
-      <c r="W87" s="12"/>
-    </row>
-    <row r="88" spans="22:23">
-      <c r="V88" s="12"/>
-      <c r="W88" s="12"/>
-    </row>
-    <row r="89" spans="22:23">
-      <c r="V89" s="12"/>
-      <c r="W89" s="12"/>
-    </row>
-    <row r="90" spans="22:23">
-      <c r="V90" s="12"/>
-      <c r="W90" s="12"/>
-    </row>
-    <row r="91" spans="22:23">
-      <c r="V91" s="12"/>
-      <c r="W91" s="12"/>
-    </row>
-    <row r="92" spans="22:23">
-      <c r="V92" s="12"/>
-      <c r="W92" s="12"/>
-    </row>
-    <row r="93" spans="22:23">
-      <c r="V93" s="12"/>
-      <c r="W93" s="12"/>
-    </row>
-    <row r="94" spans="22:23">
-      <c r="V94" s="12"/>
-      <c r="W94" s="12"/>
-    </row>
-    <row r="95" spans="22:23">
-      <c r="V95" s="12"/>
-      <c r="W95" s="12"/>
-    </row>
-    <row r="96" spans="22:23">
-      <c r="V96" s="12"/>
-      <c r="W96" s="12"/>
-    </row>
-    <row r="97" spans="22:23">
-      <c r="V97" s="12"/>
-      <c r="W97" s="12"/>
-    </row>
-    <row r="98" spans="22:23">
-      <c r="V98" s="12"/>
-      <c r="W98" s="12"/>
-    </row>
-    <row r="99" spans="22:23">
-      <c r="V99" s="12"/>
-      <c r="W99" s="12"/>
-    </row>
-    <row r="100" spans="22:23">
-      <c r="V100" s="12"/>
-      <c r="W100" s="12"/>
-    </row>
-    <row r="101" spans="22:23">
-      <c r="V101" s="12"/>
-      <c r="W101" s="12"/>
-    </row>
-    <row r="102" spans="22:23">
-      <c r="V102" s="12"/>
-      <c r="W102" s="12"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>